<commit_message>
PH - Doplněno o sloupce pro vytežené hodnoty
</commit_message>
<xml_diff>
--- a/data/DataSet_vyplněný.xlsx
+++ b/data/DataSet_vyplněný.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hladilpet\Documents\UiPath\PPP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DDE406-0337-4B69-83F1-868E6D11E866}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7090861-9CB5-4878-84AF-6E6309ED1C4D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vstupniData" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="611">
   <si>
     <t>No.</t>
   </si>
@@ -1835,6 +1835,48 @@
   </si>
   <si>
     <t>cisloZOP</t>
+  </si>
+  <si>
+    <t>stav procesu 1</t>
+  </si>
+  <si>
+    <t>stav procesu2</t>
+  </si>
+  <si>
+    <t>stav procesu3</t>
+  </si>
+  <si>
+    <t>Doplnění1</t>
+  </si>
+  <si>
+    <t>Doplněni 2</t>
+  </si>
+  <si>
+    <t>doplneni 3</t>
+  </si>
+  <si>
+    <t>doplneni 4</t>
+  </si>
+  <si>
+    <t>Jméno + příjmení</t>
+  </si>
+  <si>
+    <t>Adresa</t>
+  </si>
+  <si>
+    <t>Datum narození</t>
+  </si>
+  <si>
+    <t>Číslo OP</t>
+  </si>
+  <si>
+    <t>HJ</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t>Výsledek zpracování</t>
   </si>
 </sst>
 </file>
@@ -1869,7 +1911,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1888,8 +1930,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1912,12 +1966,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1939,6 +2004,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
@@ -2237,10 +2308,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:S168"/>
+  <dimension ref="A1:AH168"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC7" sqref="A1:AC7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2263,9 +2334,12 @@
     <col min="17" max="17" width="41" customWidth="1"/>
     <col min="18" max="18" width="34.5703125" customWidth="1"/>
     <col min="19" max="19" width="31.85546875" customWidth="1"/>
+    <col min="20" max="21" width="10.140625" customWidth="1"/>
+    <col min="22" max="22" width="7.28515625" customWidth="1"/>
+    <col min="23" max="34" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2323,8 +2397,51 @@
       <c r="S1" s="4" t="s">
         <v>572</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" s="18" t="s">
+        <v>600</v>
+      </c>
+      <c r="U1" s="18" t="s">
+        <v>601</v>
+      </c>
+      <c r="V1" s="18" t="s">
+        <v>602</v>
+      </c>
+      <c r="W1" s="18" t="s">
+        <v>603</v>
+      </c>
+      <c r="X1" s="21" t="s">
+        <v>604</v>
+      </c>
+      <c r="Y1" s="21" t="s">
+        <v>605</v>
+      </c>
+      <c r="Z1" s="21" t="s">
+        <v>606</v>
+      </c>
+      <c r="AA1" s="21" t="s">
+        <v>607</v>
+      </c>
+      <c r="AB1" s="21" t="s">
+        <v>608</v>
+      </c>
+      <c r="AC1" s="21" t="s">
+        <v>609</v>
+      </c>
+      <c r="AD1" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="AE1" s="17" t="s">
+        <v>598</v>
+      </c>
+      <c r="AF1" s="17" t="s">
+        <v>599</v>
+      </c>
+      <c r="AG1" s="22" t="s">
+        <v>610</v>
+      </c>
+      <c r="AH1" s="18"/>
+    </row>
+    <row r="2" spans="1:34" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <f>IF(C2&lt;&gt;"",1,"")</f>
         <v>1</v>
@@ -2389,8 +2506,23 @@
       <c r="S2" s="6">
         <v>777875678</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="19"/>
+      <c r="AC2" s="19"/>
+      <c r="AD2" s="19"/>
+      <c r="AE2" s="19"/>
+      <c r="AF2" s="19"/>
+      <c r="AG2" s="19"/>
+      <c r="AH2" s="19"/>
+    </row>
+    <row r="3" spans="1:34" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <f>IF(C3&lt;&gt;"",A2+1,"")</f>
         <v>2</v>
@@ -2455,8 +2587,23 @@
       <c r="S3" s="6">
         <v>603283816</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T3" s="19"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="19"/>
+      <c r="W3" s="19"/>
+      <c r="X3" s="19"/>
+      <c r="Y3" s="19"/>
+      <c r="Z3" s="19"/>
+      <c r="AA3" s="19"/>
+      <c r="AB3" s="19"/>
+      <c r="AC3" s="19"/>
+      <c r="AD3" s="19"/>
+      <c r="AE3" s="19"/>
+      <c r="AF3" s="19"/>
+      <c r="AG3" s="19"/>
+      <c r="AH3" s="19"/>
+    </row>
+    <row r="4" spans="1:34" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <f t="shared" ref="A4:A8" si="2">IF(C4&lt;&gt;"",A3+1,"")</f>
         <v>3</v>
@@ -2521,8 +2668,23 @@
       <c r="S4" s="6">
         <v>777232251</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="19"/>
+      <c r="X4" s="19"/>
+      <c r="Y4" s="19"/>
+      <c r="Z4" s="19"/>
+      <c r="AA4" s="19"/>
+      <c r="AB4" s="19"/>
+      <c r="AC4" s="19"/>
+      <c r="AD4" s="19"/>
+      <c r="AE4" s="19"/>
+      <c r="AF4" s="19"/>
+      <c r="AG4" s="19"/>
+      <c r="AH4" s="19"/>
+    </row>
+    <row r="5" spans="1:34" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -2587,8 +2749,23 @@
       <c r="S5" s="6">
         <v>606655037</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="19"/>
+      <c r="X5" s="19"/>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19"/>
+      <c r="AA5" s="19"/>
+      <c r="AB5" s="19"/>
+      <c r="AC5" s="19"/>
+      <c r="AD5" s="19"/>
+      <c r="AE5" s="19"/>
+      <c r="AF5" s="19"/>
+      <c r="AG5" s="19"/>
+      <c r="AH5" s="19"/>
+    </row>
+    <row r="6" spans="1:34" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -2653,8 +2830,23 @@
       <c r="S6" s="6">
         <v>603781363</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="19"/>
+      <c r="X6" s="19"/>
+      <c r="Y6" s="19"/>
+      <c r="Z6" s="19"/>
+      <c r="AA6" s="19"/>
+      <c r="AB6" s="19"/>
+      <c r="AC6" s="19"/>
+      <c r="AD6" s="19"/>
+      <c r="AE6" s="19"/>
+      <c r="AF6" s="19"/>
+      <c r="AG6" s="19"/>
+      <c r="AH6" s="19"/>
+    </row>
+    <row r="7" spans="1:34" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2677,8 +2869,23 @@
       <c r="Q7" s="14"/>
       <c r="R7" s="14"/>
       <c r="S7" s="14"/>
-    </row>
-    <row r="8" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="19"/>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="19"/>
+      <c r="Z7" s="19"/>
+      <c r="AA7" s="19"/>
+      <c r="AB7" s="19"/>
+      <c r="AC7" s="19"/>
+      <c r="AD7" s="19"/>
+      <c r="AE7" s="19"/>
+      <c r="AF7" s="19"/>
+      <c r="AG7" s="19"/>
+      <c r="AH7" s="19"/>
+    </row>
+    <row r="8" spans="1:34" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2701,8 +2908,23 @@
       <c r="Q8" s="14"/>
       <c r="R8" s="14"/>
       <c r="S8" s="14"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T8" s="19"/>
+      <c r="U8" s="19"/>
+      <c r="V8" s="19"/>
+      <c r="W8" s="19"/>
+      <c r="X8" s="19"/>
+      <c r="Y8" s="19"/>
+      <c r="Z8" s="19"/>
+      <c r="AA8" s="19"/>
+      <c r="AB8" s="19"/>
+      <c r="AC8" s="19"/>
+      <c r="AD8" s="19"/>
+      <c r="AE8" s="19"/>
+      <c r="AF8" s="19"/>
+      <c r="AG8" s="19"/>
+      <c r="AH8" s="19"/>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="str">
         <f>IF(C9&lt;&gt;"",#REF!+1,"")</f>
         <v/>
@@ -2743,8 +2965,23 @@
         <v/>
       </c>
       <c r="S9" s="4"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T9" s="20"/>
+      <c r="U9" s="20"/>
+      <c r="V9" s="20"/>
+      <c r="W9" s="20"/>
+      <c r="X9" s="20"/>
+      <c r="Y9" s="20"/>
+      <c r="Z9" s="20"/>
+      <c r="AA9" s="20"/>
+      <c r="AB9" s="20"/>
+      <c r="AC9" s="20"/>
+      <c r="AD9" s="20"/>
+      <c r="AE9" s="20"/>
+      <c r="AF9" s="20"/>
+      <c r="AG9" s="20"/>
+      <c r="AH9" s="20"/>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="str">
         <f t="shared" ref="A10:A66" si="5">IF(C10&lt;&gt;"",A9+1,"")</f>
         <v/>
@@ -2785,8 +3022,23 @@
         <v/>
       </c>
       <c r="S10" s="4"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T10" s="20"/>
+      <c r="U10" s="20"/>
+      <c r="V10" s="20"/>
+      <c r="W10" s="20"/>
+      <c r="X10" s="20"/>
+      <c r="Y10" s="20"/>
+      <c r="Z10" s="20"/>
+      <c r="AA10" s="20"/>
+      <c r="AB10" s="20"/>
+      <c r="AC10" s="20"/>
+      <c r="AD10" s="20"/>
+      <c r="AE10" s="20"/>
+      <c r="AF10" s="20"/>
+      <c r="AG10" s="20"/>
+      <c r="AH10" s="20"/>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -2827,8 +3079,23 @@
         <v/>
       </c>
       <c r="S11" s="4"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T11" s="20"/>
+      <c r="U11" s="20"/>
+      <c r="V11" s="20"/>
+      <c r="W11" s="20"/>
+      <c r="X11" s="20"/>
+      <c r="Y11" s="20"/>
+      <c r="Z11" s="20"/>
+      <c r="AA11" s="20"/>
+      <c r="AB11" s="20"/>
+      <c r="AC11" s="20"/>
+      <c r="AD11" s="20"/>
+      <c r="AE11" s="20"/>
+      <c r="AF11" s="20"/>
+      <c r="AG11" s="20"/>
+      <c r="AH11" s="20"/>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -2869,8 +3136,23 @@
         <v/>
       </c>
       <c r="S12" s="4"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T12" s="20"/>
+      <c r="U12" s="20"/>
+      <c r="V12" s="20"/>
+      <c r="W12" s="20"/>
+      <c r="X12" s="20"/>
+      <c r="Y12" s="20"/>
+      <c r="Z12" s="20"/>
+      <c r="AA12" s="20"/>
+      <c r="AB12" s="20"/>
+      <c r="AC12" s="20"/>
+      <c r="AD12" s="20"/>
+      <c r="AE12" s="20"/>
+      <c r="AF12" s="20"/>
+      <c r="AG12" s="20"/>
+      <c r="AH12" s="20"/>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -2911,8 +3193,23 @@
         <v/>
       </c>
       <c r="S13" s="4"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T13" s="20"/>
+      <c r="U13" s="20"/>
+      <c r="V13" s="20"/>
+      <c r="W13" s="20"/>
+      <c r="X13" s="20"/>
+      <c r="Y13" s="20"/>
+      <c r="Z13" s="20"/>
+      <c r="AA13" s="20"/>
+      <c r="AB13" s="20"/>
+      <c r="AC13" s="20"/>
+      <c r="AD13" s="20"/>
+      <c r="AE13" s="20"/>
+      <c r="AF13" s="20"/>
+      <c r="AG13" s="20"/>
+      <c r="AH13" s="20"/>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -2953,8 +3250,23 @@
         <v/>
       </c>
       <c r="S14" s="4"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T14" s="20"/>
+      <c r="U14" s="20"/>
+      <c r="V14" s="20"/>
+      <c r="W14" s="20"/>
+      <c r="X14" s="20"/>
+      <c r="Y14" s="20"/>
+      <c r="Z14" s="20"/>
+      <c r="AA14" s="20"/>
+      <c r="AB14" s="20"/>
+      <c r="AC14" s="20"/>
+      <c r="AD14" s="20"/>
+      <c r="AE14" s="20"/>
+      <c r="AF14" s="20"/>
+      <c r="AG14" s="20"/>
+      <c r="AH14" s="20"/>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -2995,8 +3307,23 @@
         <v/>
       </c>
       <c r="S15" s="4"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T15" s="20"/>
+      <c r="U15" s="20"/>
+      <c r="V15" s="20"/>
+      <c r="W15" s="20"/>
+      <c r="X15" s="20"/>
+      <c r="Y15" s="20"/>
+      <c r="Z15" s="20"/>
+      <c r="AA15" s="20"/>
+      <c r="AB15" s="20"/>
+      <c r="AC15" s="20"/>
+      <c r="AD15" s="20"/>
+      <c r="AE15" s="20"/>
+      <c r="AF15" s="20"/>
+      <c r="AG15" s="20"/>
+      <c r="AH15" s="20"/>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3037,8 +3364,23 @@
         <v/>
       </c>
       <c r="S16" s="4"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T16" s="20"/>
+      <c r="U16" s="20"/>
+      <c r="V16" s="20"/>
+      <c r="W16" s="20"/>
+      <c r="X16" s="20"/>
+      <c r="Y16" s="20"/>
+      <c r="Z16" s="20"/>
+      <c r="AA16" s="20"/>
+      <c r="AB16" s="20"/>
+      <c r="AC16" s="20"/>
+      <c r="AD16" s="20"/>
+      <c r="AE16" s="20"/>
+      <c r="AF16" s="20"/>
+      <c r="AG16" s="20"/>
+      <c r="AH16" s="20"/>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3079,8 +3421,23 @@
         <v/>
       </c>
       <c r="S17" s="4"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T17" s="20"/>
+      <c r="U17" s="20"/>
+      <c r="V17" s="20"/>
+      <c r="W17" s="20"/>
+      <c r="X17" s="20"/>
+      <c r="Y17" s="20"/>
+      <c r="Z17" s="20"/>
+      <c r="AA17" s="20"/>
+      <c r="AB17" s="20"/>
+      <c r="AC17" s="20"/>
+      <c r="AD17" s="20"/>
+      <c r="AE17" s="20"/>
+      <c r="AF17" s="20"/>
+      <c r="AG17" s="20"/>
+      <c r="AH17" s="20"/>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3121,8 +3478,23 @@
         <v/>
       </c>
       <c r="S18" s="4"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T18" s="20"/>
+      <c r="U18" s="20"/>
+      <c r="V18" s="20"/>
+      <c r="W18" s="20"/>
+      <c r="X18" s="20"/>
+      <c r="Y18" s="20"/>
+      <c r="Z18" s="20"/>
+      <c r="AA18" s="20"/>
+      <c r="AB18" s="20"/>
+      <c r="AC18" s="20"/>
+      <c r="AD18" s="20"/>
+      <c r="AE18" s="20"/>
+      <c r="AF18" s="20"/>
+      <c r="AG18" s="20"/>
+      <c r="AH18" s="20"/>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3163,8 +3535,23 @@
         <v/>
       </c>
       <c r="S19" s="4"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T19" s="20"/>
+      <c r="U19" s="20"/>
+      <c r="V19" s="20"/>
+      <c r="W19" s="20"/>
+      <c r="X19" s="20"/>
+      <c r="Y19" s="20"/>
+      <c r="Z19" s="20"/>
+      <c r="AA19" s="20"/>
+      <c r="AB19" s="20"/>
+      <c r="AC19" s="20"/>
+      <c r="AD19" s="20"/>
+      <c r="AE19" s="20"/>
+      <c r="AF19" s="20"/>
+      <c r="AG19" s="20"/>
+      <c r="AH19" s="20"/>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3205,8 +3592,23 @@
         <v/>
       </c>
       <c r="S20" s="4"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T20" s="20"/>
+      <c r="U20" s="20"/>
+      <c r="V20" s="20"/>
+      <c r="W20" s="20"/>
+      <c r="X20" s="20"/>
+      <c r="Y20" s="20"/>
+      <c r="Z20" s="20"/>
+      <c r="AA20" s="20"/>
+      <c r="AB20" s="20"/>
+      <c r="AC20" s="20"/>
+      <c r="AD20" s="20"/>
+      <c r="AE20" s="20"/>
+      <c r="AF20" s="20"/>
+      <c r="AG20" s="20"/>
+      <c r="AH20" s="20"/>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3247,8 +3649,23 @@
         <v/>
       </c>
       <c r="S21" s="4"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T21" s="20"/>
+      <c r="U21" s="20"/>
+      <c r="V21" s="20"/>
+      <c r="W21" s="20"/>
+      <c r="X21" s="20"/>
+      <c r="Y21" s="20"/>
+      <c r="Z21" s="20"/>
+      <c r="AA21" s="20"/>
+      <c r="AB21" s="20"/>
+      <c r="AC21" s="20"/>
+      <c r="AD21" s="20"/>
+      <c r="AE21" s="20"/>
+      <c r="AF21" s="20"/>
+      <c r="AG21" s="20"/>
+      <c r="AH21" s="20"/>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3289,8 +3706,23 @@
         <v/>
       </c>
       <c r="S22" s="4"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T22" s="20"/>
+      <c r="U22" s="20"/>
+      <c r="V22" s="20"/>
+      <c r="W22" s="20"/>
+      <c r="X22" s="20"/>
+      <c r="Y22" s="20"/>
+      <c r="Z22" s="20"/>
+      <c r="AA22" s="20"/>
+      <c r="AB22" s="20"/>
+      <c r="AC22" s="20"/>
+      <c r="AD22" s="20"/>
+      <c r="AE22" s="20"/>
+      <c r="AF22" s="20"/>
+      <c r="AG22" s="20"/>
+      <c r="AH22" s="20"/>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3331,8 +3763,23 @@
         <v/>
       </c>
       <c r="S23" s="4"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T23" s="20"/>
+      <c r="U23" s="20"/>
+      <c r="V23" s="20"/>
+      <c r="W23" s="20"/>
+      <c r="X23" s="20"/>
+      <c r="Y23" s="20"/>
+      <c r="Z23" s="20"/>
+      <c r="AA23" s="20"/>
+      <c r="AB23" s="20"/>
+      <c r="AC23" s="20"/>
+      <c r="AD23" s="20"/>
+      <c r="AE23" s="20"/>
+      <c r="AF23" s="20"/>
+      <c r="AG23" s="20"/>
+      <c r="AH23" s="20"/>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3373,8 +3820,23 @@
         <v/>
       </c>
       <c r="S24" s="4"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T24" s="20"/>
+      <c r="U24" s="20"/>
+      <c r="V24" s="20"/>
+      <c r="W24" s="20"/>
+      <c r="X24" s="20"/>
+      <c r="Y24" s="20"/>
+      <c r="Z24" s="20"/>
+      <c r="AA24" s="20"/>
+      <c r="AB24" s="20"/>
+      <c r="AC24" s="20"/>
+      <c r="AD24" s="20"/>
+      <c r="AE24" s="20"/>
+      <c r="AF24" s="20"/>
+      <c r="AG24" s="20"/>
+      <c r="AH24" s="20"/>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3415,8 +3877,23 @@
         <v/>
       </c>
       <c r="S25" s="4"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T25" s="20"/>
+      <c r="U25" s="20"/>
+      <c r="V25" s="20"/>
+      <c r="W25" s="20"/>
+      <c r="X25" s="20"/>
+      <c r="Y25" s="20"/>
+      <c r="Z25" s="20"/>
+      <c r="AA25" s="20"/>
+      <c r="AB25" s="20"/>
+      <c r="AC25" s="20"/>
+      <c r="AD25" s="20"/>
+      <c r="AE25" s="20"/>
+      <c r="AF25" s="20"/>
+      <c r="AG25" s="20"/>
+      <c r="AH25" s="20"/>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3457,8 +3934,23 @@
         <v/>
       </c>
       <c r="S26" s="4"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T26" s="20"/>
+      <c r="U26" s="20"/>
+      <c r="V26" s="20"/>
+      <c r="W26" s="20"/>
+      <c r="X26" s="20"/>
+      <c r="Y26" s="20"/>
+      <c r="Z26" s="20"/>
+      <c r="AA26" s="20"/>
+      <c r="AB26" s="20"/>
+      <c r="AC26" s="20"/>
+      <c r="AD26" s="20"/>
+      <c r="AE26" s="20"/>
+      <c r="AF26" s="20"/>
+      <c r="AG26" s="20"/>
+      <c r="AH26" s="20"/>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3499,8 +3991,23 @@
         <v/>
       </c>
       <c r="S27" s="4"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T27" s="20"/>
+      <c r="U27" s="20"/>
+      <c r="V27" s="20"/>
+      <c r="W27" s="20"/>
+      <c r="X27" s="20"/>
+      <c r="Y27" s="20"/>
+      <c r="Z27" s="20"/>
+      <c r="AA27" s="20"/>
+      <c r="AB27" s="20"/>
+      <c r="AC27" s="20"/>
+      <c r="AD27" s="20"/>
+      <c r="AE27" s="20"/>
+      <c r="AF27" s="20"/>
+      <c r="AG27" s="20"/>
+      <c r="AH27" s="20"/>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3541,8 +4048,23 @@
         <v/>
       </c>
       <c r="S28" s="4"/>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T28" s="20"/>
+      <c r="U28" s="20"/>
+      <c r="V28" s="20"/>
+      <c r="W28" s="20"/>
+      <c r="X28" s="20"/>
+      <c r="Y28" s="20"/>
+      <c r="Z28" s="20"/>
+      <c r="AA28" s="20"/>
+      <c r="AB28" s="20"/>
+      <c r="AC28" s="20"/>
+      <c r="AD28" s="20"/>
+      <c r="AE28" s="20"/>
+      <c r="AF28" s="20"/>
+      <c r="AG28" s="20"/>
+      <c r="AH28" s="20"/>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3583,8 +4105,23 @@
         <v/>
       </c>
       <c r="S29" s="4"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T29" s="20"/>
+      <c r="U29" s="20"/>
+      <c r="V29" s="20"/>
+      <c r="W29" s="20"/>
+      <c r="X29" s="20"/>
+      <c r="Y29" s="20"/>
+      <c r="Z29" s="20"/>
+      <c r="AA29" s="20"/>
+      <c r="AB29" s="20"/>
+      <c r="AC29" s="20"/>
+      <c r="AD29" s="20"/>
+      <c r="AE29" s="20"/>
+      <c r="AF29" s="20"/>
+      <c r="AG29" s="20"/>
+      <c r="AH29" s="20"/>
+    </row>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3625,8 +4162,23 @@
         <v/>
       </c>
       <c r="S30" s="4"/>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T30" s="20"/>
+      <c r="U30" s="20"/>
+      <c r="V30" s="20"/>
+      <c r="W30" s="20"/>
+      <c r="X30" s="20"/>
+      <c r="Y30" s="20"/>
+      <c r="Z30" s="20"/>
+      <c r="AA30" s="20"/>
+      <c r="AB30" s="20"/>
+      <c r="AC30" s="20"/>
+      <c r="AD30" s="20"/>
+      <c r="AE30" s="20"/>
+      <c r="AF30" s="20"/>
+      <c r="AG30" s="20"/>
+      <c r="AH30" s="20"/>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3667,8 +4219,23 @@
         <v/>
       </c>
       <c r="S31" s="4"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T31" s="20"/>
+      <c r="U31" s="20"/>
+      <c r="V31" s="20"/>
+      <c r="W31" s="20"/>
+      <c r="X31" s="20"/>
+      <c r="Y31" s="20"/>
+      <c r="Z31" s="20"/>
+      <c r="AA31" s="20"/>
+      <c r="AB31" s="20"/>
+      <c r="AC31" s="20"/>
+      <c r="AD31" s="20"/>
+      <c r="AE31" s="20"/>
+      <c r="AF31" s="20"/>
+      <c r="AG31" s="20"/>
+      <c r="AH31" s="20"/>
+    </row>
+    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3709,8 +4276,23 @@
         <v/>
       </c>
       <c r="S32" s="4"/>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T32" s="20"/>
+      <c r="U32" s="20"/>
+      <c r="V32" s="20"/>
+      <c r="W32" s="20"/>
+      <c r="X32" s="20"/>
+      <c r="Y32" s="20"/>
+      <c r="Z32" s="20"/>
+      <c r="AA32" s="20"/>
+      <c r="AB32" s="20"/>
+      <c r="AC32" s="20"/>
+      <c r="AD32" s="20"/>
+      <c r="AE32" s="20"/>
+      <c r="AF32" s="20"/>
+      <c r="AG32" s="20"/>
+      <c r="AH32" s="20"/>
+    </row>
+    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3751,8 +4333,23 @@
         <v/>
       </c>
       <c r="S33" s="4"/>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T33" s="20"/>
+      <c r="U33" s="20"/>
+      <c r="V33" s="20"/>
+      <c r="W33" s="20"/>
+      <c r="X33" s="20"/>
+      <c r="Y33" s="20"/>
+      <c r="Z33" s="20"/>
+      <c r="AA33" s="20"/>
+      <c r="AB33" s="20"/>
+      <c r="AC33" s="20"/>
+      <c r="AD33" s="20"/>
+      <c r="AE33" s="20"/>
+      <c r="AF33" s="20"/>
+      <c r="AG33" s="20"/>
+      <c r="AH33" s="20"/>
+    </row>
+    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3793,8 +4390,23 @@
         <v/>
       </c>
       <c r="S34" s="4"/>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T34" s="20"/>
+      <c r="U34" s="20"/>
+      <c r="V34" s="20"/>
+      <c r="W34" s="20"/>
+      <c r="X34" s="20"/>
+      <c r="Y34" s="20"/>
+      <c r="Z34" s="20"/>
+      <c r="AA34" s="20"/>
+      <c r="AB34" s="20"/>
+      <c r="AC34" s="20"/>
+      <c r="AD34" s="20"/>
+      <c r="AE34" s="20"/>
+      <c r="AF34" s="20"/>
+      <c r="AG34" s="20"/>
+      <c r="AH34" s="20"/>
+    </row>
+    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3835,8 +4447,23 @@
         <v/>
       </c>
       <c r="S35" s="4"/>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T35" s="20"/>
+      <c r="U35" s="20"/>
+      <c r="V35" s="20"/>
+      <c r="W35" s="20"/>
+      <c r="X35" s="20"/>
+      <c r="Y35" s="20"/>
+      <c r="Z35" s="20"/>
+      <c r="AA35" s="20"/>
+      <c r="AB35" s="20"/>
+      <c r="AC35" s="20"/>
+      <c r="AD35" s="20"/>
+      <c r="AE35" s="20"/>
+      <c r="AF35" s="20"/>
+      <c r="AG35" s="20"/>
+      <c r="AH35" s="20"/>
+    </row>
+    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3877,8 +4504,23 @@
         <v/>
       </c>
       <c r="S36" s="4"/>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T36" s="20"/>
+      <c r="U36" s="20"/>
+      <c r="V36" s="20"/>
+      <c r="W36" s="20"/>
+      <c r="X36" s="20"/>
+      <c r="Y36" s="20"/>
+      <c r="Z36" s="20"/>
+      <c r="AA36" s="20"/>
+      <c r="AB36" s="20"/>
+      <c r="AC36" s="20"/>
+      <c r="AD36" s="20"/>
+      <c r="AE36" s="20"/>
+      <c r="AF36" s="20"/>
+      <c r="AG36" s="20"/>
+      <c r="AH36" s="20"/>
+    </row>
+    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3919,8 +4561,23 @@
         <v/>
       </c>
       <c r="S37" s="4"/>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T37" s="20"/>
+      <c r="U37" s="20"/>
+      <c r="V37" s="20"/>
+      <c r="W37" s="20"/>
+      <c r="X37" s="20"/>
+      <c r="Y37" s="20"/>
+      <c r="Z37" s="20"/>
+      <c r="AA37" s="20"/>
+      <c r="AB37" s="20"/>
+      <c r="AC37" s="20"/>
+      <c r="AD37" s="20"/>
+      <c r="AE37" s="20"/>
+      <c r="AF37" s="20"/>
+      <c r="AG37" s="20"/>
+      <c r="AH37" s="20"/>
+    </row>
+    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3961,8 +4618,23 @@
         <v/>
       </c>
       <c r="S38" s="4"/>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T38" s="20"/>
+      <c r="U38" s="20"/>
+      <c r="V38" s="20"/>
+      <c r="W38" s="20"/>
+      <c r="X38" s="20"/>
+      <c r="Y38" s="20"/>
+      <c r="Z38" s="20"/>
+      <c r="AA38" s="20"/>
+      <c r="AB38" s="20"/>
+      <c r="AC38" s="20"/>
+      <c r="AD38" s="20"/>
+      <c r="AE38" s="20"/>
+      <c r="AF38" s="20"/>
+      <c r="AG38" s="20"/>
+      <c r="AH38" s="20"/>
+    </row>
+    <row r="39" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4003,8 +4675,23 @@
         <v/>
       </c>
       <c r="S39" s="4"/>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T39" s="20"/>
+      <c r="U39" s="20"/>
+      <c r="V39" s="20"/>
+      <c r="W39" s="20"/>
+      <c r="X39" s="20"/>
+      <c r="Y39" s="20"/>
+      <c r="Z39" s="20"/>
+      <c r="AA39" s="20"/>
+      <c r="AB39" s="20"/>
+      <c r="AC39" s="20"/>
+      <c r="AD39" s="20"/>
+      <c r="AE39" s="20"/>
+      <c r="AF39" s="20"/>
+      <c r="AG39" s="20"/>
+      <c r="AH39" s="20"/>
+    </row>
+    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4045,8 +4732,23 @@
         <v/>
       </c>
       <c r="S40" s="4"/>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T40" s="20"/>
+      <c r="U40" s="20"/>
+      <c r="V40" s="20"/>
+      <c r="W40" s="20"/>
+      <c r="X40" s="20"/>
+      <c r="Y40" s="20"/>
+      <c r="Z40" s="20"/>
+      <c r="AA40" s="20"/>
+      <c r="AB40" s="20"/>
+      <c r="AC40" s="20"/>
+      <c r="AD40" s="20"/>
+      <c r="AE40" s="20"/>
+      <c r="AF40" s="20"/>
+      <c r="AG40" s="20"/>
+      <c r="AH40" s="20"/>
+    </row>
+    <row r="41" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4087,8 +4789,23 @@
         <v/>
       </c>
       <c r="S41" s="4"/>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T41" s="20"/>
+      <c r="U41" s="20"/>
+      <c r="V41" s="20"/>
+      <c r="W41" s="20"/>
+      <c r="X41" s="20"/>
+      <c r="Y41" s="20"/>
+      <c r="Z41" s="20"/>
+      <c r="AA41" s="20"/>
+      <c r="AB41" s="20"/>
+      <c r="AC41" s="20"/>
+      <c r="AD41" s="20"/>
+      <c r="AE41" s="20"/>
+      <c r="AF41" s="20"/>
+      <c r="AG41" s="20"/>
+      <c r="AH41" s="20"/>
+    </row>
+    <row r="42" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4129,8 +4846,23 @@
         <v/>
       </c>
       <c r="S42" s="4"/>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T42" s="20"/>
+      <c r="U42" s="20"/>
+      <c r="V42" s="20"/>
+      <c r="W42" s="20"/>
+      <c r="X42" s="20"/>
+      <c r="Y42" s="20"/>
+      <c r="Z42" s="20"/>
+      <c r="AA42" s="20"/>
+      <c r="AB42" s="20"/>
+      <c r="AC42" s="20"/>
+      <c r="AD42" s="20"/>
+      <c r="AE42" s="20"/>
+      <c r="AF42" s="20"/>
+      <c r="AG42" s="20"/>
+      <c r="AH42" s="20"/>
+    </row>
+    <row r="43" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4171,8 +4903,23 @@
         <v/>
       </c>
       <c r="S43" s="4"/>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T43" s="20"/>
+      <c r="U43" s="20"/>
+      <c r="V43" s="20"/>
+      <c r="W43" s="20"/>
+      <c r="X43" s="20"/>
+      <c r="Y43" s="20"/>
+      <c r="Z43" s="20"/>
+      <c r="AA43" s="20"/>
+      <c r="AB43" s="20"/>
+      <c r="AC43" s="20"/>
+      <c r="AD43" s="20"/>
+      <c r="AE43" s="20"/>
+      <c r="AF43" s="20"/>
+      <c r="AG43" s="20"/>
+      <c r="AH43" s="20"/>
+    </row>
+    <row r="44" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4213,8 +4960,23 @@
         <v/>
       </c>
       <c r="S44" s="4"/>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T44" s="20"/>
+      <c r="U44" s="20"/>
+      <c r="V44" s="20"/>
+      <c r="W44" s="20"/>
+      <c r="X44" s="20"/>
+      <c r="Y44" s="20"/>
+      <c r="Z44" s="20"/>
+      <c r="AA44" s="20"/>
+      <c r="AB44" s="20"/>
+      <c r="AC44" s="20"/>
+      <c r="AD44" s="20"/>
+      <c r="AE44" s="20"/>
+      <c r="AF44" s="20"/>
+      <c r="AG44" s="20"/>
+      <c r="AH44" s="20"/>
+    </row>
+    <row r="45" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4255,8 +5017,23 @@
         <v/>
       </c>
       <c r="S45" s="4"/>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T45" s="20"/>
+      <c r="U45" s="20"/>
+      <c r="V45" s="20"/>
+      <c r="W45" s="20"/>
+      <c r="X45" s="20"/>
+      <c r="Y45" s="20"/>
+      <c r="Z45" s="20"/>
+      <c r="AA45" s="20"/>
+      <c r="AB45" s="20"/>
+      <c r="AC45" s="20"/>
+      <c r="AD45" s="20"/>
+      <c r="AE45" s="20"/>
+      <c r="AF45" s="20"/>
+      <c r="AG45" s="20"/>
+      <c r="AH45" s="20"/>
+    </row>
+    <row r="46" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4297,8 +5074,23 @@
         <v/>
       </c>
       <c r="S46" s="4"/>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T46" s="20"/>
+      <c r="U46" s="20"/>
+      <c r="V46" s="20"/>
+      <c r="W46" s="20"/>
+      <c r="X46" s="20"/>
+      <c r="Y46" s="20"/>
+      <c r="Z46" s="20"/>
+      <c r="AA46" s="20"/>
+      <c r="AB46" s="20"/>
+      <c r="AC46" s="20"/>
+      <c r="AD46" s="20"/>
+      <c r="AE46" s="20"/>
+      <c r="AF46" s="20"/>
+      <c r="AG46" s="20"/>
+      <c r="AH46" s="20"/>
+    </row>
+    <row r="47" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4339,8 +5131,23 @@
         <v/>
       </c>
       <c r="S47" s="4"/>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T47" s="20"/>
+      <c r="U47" s="20"/>
+      <c r="V47" s="20"/>
+      <c r="W47" s="20"/>
+      <c r="X47" s="20"/>
+      <c r="Y47" s="20"/>
+      <c r="Z47" s="20"/>
+      <c r="AA47" s="20"/>
+      <c r="AB47" s="20"/>
+      <c r="AC47" s="20"/>
+      <c r="AD47" s="20"/>
+      <c r="AE47" s="20"/>
+      <c r="AF47" s="20"/>
+      <c r="AG47" s="20"/>
+      <c r="AH47" s="20"/>
+    </row>
+    <row r="48" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4381,8 +5188,23 @@
         <v/>
       </c>
       <c r="S48" s="4"/>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T48" s="20"/>
+      <c r="U48" s="20"/>
+      <c r="V48" s="20"/>
+      <c r="W48" s="20"/>
+      <c r="X48" s="20"/>
+      <c r="Y48" s="20"/>
+      <c r="Z48" s="20"/>
+      <c r="AA48" s="20"/>
+      <c r="AB48" s="20"/>
+      <c r="AC48" s="20"/>
+      <c r="AD48" s="20"/>
+      <c r="AE48" s="20"/>
+      <c r="AF48" s="20"/>
+      <c r="AG48" s="20"/>
+      <c r="AH48" s="20"/>
+    </row>
+    <row r="49" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4423,8 +5245,23 @@
         <v/>
       </c>
       <c r="S49" s="4"/>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T49" s="20"/>
+      <c r="U49" s="20"/>
+      <c r="V49" s="20"/>
+      <c r="W49" s="20"/>
+      <c r="X49" s="20"/>
+      <c r="Y49" s="20"/>
+      <c r="Z49" s="20"/>
+      <c r="AA49" s="20"/>
+      <c r="AB49" s="20"/>
+      <c r="AC49" s="20"/>
+      <c r="AD49" s="20"/>
+      <c r="AE49" s="20"/>
+      <c r="AF49" s="20"/>
+      <c r="AG49" s="20"/>
+      <c r="AH49" s="20"/>
+    </row>
+    <row r="50" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4465,8 +5302,23 @@
         <v/>
       </c>
       <c r="S50" s="4"/>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T50" s="20"/>
+      <c r="U50" s="20"/>
+      <c r="V50" s="20"/>
+      <c r="W50" s="20"/>
+      <c r="X50" s="20"/>
+      <c r="Y50" s="20"/>
+      <c r="Z50" s="20"/>
+      <c r="AA50" s="20"/>
+      <c r="AB50" s="20"/>
+      <c r="AC50" s="20"/>
+      <c r="AD50" s="20"/>
+      <c r="AE50" s="20"/>
+      <c r="AF50" s="20"/>
+      <c r="AG50" s="20"/>
+      <c r="AH50" s="20"/>
+    </row>
+    <row r="51" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4507,8 +5359,23 @@
         <v/>
       </c>
       <c r="S51" s="4"/>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T51" s="20"/>
+      <c r="U51" s="20"/>
+      <c r="V51" s="20"/>
+      <c r="W51" s="20"/>
+      <c r="X51" s="20"/>
+      <c r="Y51" s="20"/>
+      <c r="Z51" s="20"/>
+      <c r="AA51" s="20"/>
+      <c r="AB51" s="20"/>
+      <c r="AC51" s="20"/>
+      <c r="AD51" s="20"/>
+      <c r="AE51" s="20"/>
+      <c r="AF51" s="20"/>
+      <c r="AG51" s="20"/>
+      <c r="AH51" s="20"/>
+    </row>
+    <row r="52" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4549,8 +5416,23 @@
         <v/>
       </c>
       <c r="S52" s="4"/>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T52" s="20"/>
+      <c r="U52" s="20"/>
+      <c r="V52" s="20"/>
+      <c r="W52" s="20"/>
+      <c r="X52" s="20"/>
+      <c r="Y52" s="20"/>
+      <c r="Z52" s="20"/>
+      <c r="AA52" s="20"/>
+      <c r="AB52" s="20"/>
+      <c r="AC52" s="20"/>
+      <c r="AD52" s="20"/>
+      <c r="AE52" s="20"/>
+      <c r="AF52" s="20"/>
+      <c r="AG52" s="20"/>
+      <c r="AH52" s="20"/>
+    </row>
+    <row r="53" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4591,8 +5473,23 @@
         <v/>
       </c>
       <c r="S53" s="4"/>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T53" s="20"/>
+      <c r="U53" s="20"/>
+      <c r="V53" s="20"/>
+      <c r="W53" s="20"/>
+      <c r="X53" s="20"/>
+      <c r="Y53" s="20"/>
+      <c r="Z53" s="20"/>
+      <c r="AA53" s="20"/>
+      <c r="AB53" s="20"/>
+      <c r="AC53" s="20"/>
+      <c r="AD53" s="20"/>
+      <c r="AE53" s="20"/>
+      <c r="AF53" s="20"/>
+      <c r="AG53" s="20"/>
+      <c r="AH53" s="20"/>
+    </row>
+    <row r="54" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4633,8 +5530,23 @@
         <v/>
       </c>
       <c r="S54" s="4"/>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T54" s="20"/>
+      <c r="U54" s="20"/>
+      <c r="V54" s="20"/>
+      <c r="W54" s="20"/>
+      <c r="X54" s="20"/>
+      <c r="Y54" s="20"/>
+      <c r="Z54" s="20"/>
+      <c r="AA54" s="20"/>
+      <c r="AB54" s="20"/>
+      <c r="AC54" s="20"/>
+      <c r="AD54" s="20"/>
+      <c r="AE54" s="20"/>
+      <c r="AF54" s="20"/>
+      <c r="AG54" s="20"/>
+      <c r="AH54" s="20"/>
+    </row>
+    <row r="55" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4675,8 +5587,23 @@
         <v/>
       </c>
       <c r="S55" s="4"/>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T55" s="20"/>
+      <c r="U55" s="20"/>
+      <c r="V55" s="20"/>
+      <c r="W55" s="20"/>
+      <c r="X55" s="20"/>
+      <c r="Y55" s="20"/>
+      <c r="Z55" s="20"/>
+      <c r="AA55" s="20"/>
+      <c r="AB55" s="20"/>
+      <c r="AC55" s="20"/>
+      <c r="AD55" s="20"/>
+      <c r="AE55" s="20"/>
+      <c r="AF55" s="20"/>
+      <c r="AG55" s="20"/>
+      <c r="AH55" s="20"/>
+    </row>
+    <row r="56" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4717,8 +5644,23 @@
         <v/>
       </c>
       <c r="S56" s="4"/>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T56" s="20"/>
+      <c r="U56" s="20"/>
+      <c r="V56" s="20"/>
+      <c r="W56" s="20"/>
+      <c r="X56" s="20"/>
+      <c r="Y56" s="20"/>
+      <c r="Z56" s="20"/>
+      <c r="AA56" s="20"/>
+      <c r="AB56" s="20"/>
+      <c r="AC56" s="20"/>
+      <c r="AD56" s="20"/>
+      <c r="AE56" s="20"/>
+      <c r="AF56" s="20"/>
+      <c r="AG56" s="20"/>
+      <c r="AH56" s="20"/>
+    </row>
+    <row r="57" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4759,8 +5701,23 @@
         <v/>
       </c>
       <c r="S57" s="4"/>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T57" s="20"/>
+      <c r="U57" s="20"/>
+      <c r="V57" s="20"/>
+      <c r="W57" s="20"/>
+      <c r="X57" s="20"/>
+      <c r="Y57" s="20"/>
+      <c r="Z57" s="20"/>
+      <c r="AA57" s="20"/>
+      <c r="AB57" s="20"/>
+      <c r="AC57" s="20"/>
+      <c r="AD57" s="20"/>
+      <c r="AE57" s="20"/>
+      <c r="AF57" s="20"/>
+      <c r="AG57" s="20"/>
+      <c r="AH57" s="20"/>
+    </row>
+    <row r="58" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4801,8 +5758,23 @@
         <v/>
       </c>
       <c r="S58" s="4"/>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T58" s="20"/>
+      <c r="U58" s="20"/>
+      <c r="V58" s="20"/>
+      <c r="W58" s="20"/>
+      <c r="X58" s="20"/>
+      <c r="Y58" s="20"/>
+      <c r="Z58" s="20"/>
+      <c r="AA58" s="20"/>
+      <c r="AB58" s="20"/>
+      <c r="AC58" s="20"/>
+      <c r="AD58" s="20"/>
+      <c r="AE58" s="20"/>
+      <c r="AF58" s="20"/>
+      <c r="AG58" s="20"/>
+      <c r="AH58" s="20"/>
+    </row>
+    <row r="59" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4843,8 +5815,23 @@
         <v/>
       </c>
       <c r="S59" s="4"/>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T59" s="20"/>
+      <c r="U59" s="20"/>
+      <c r="V59" s="20"/>
+      <c r="W59" s="20"/>
+      <c r="X59" s="20"/>
+      <c r="Y59" s="20"/>
+      <c r="Z59" s="20"/>
+      <c r="AA59" s="20"/>
+      <c r="AB59" s="20"/>
+      <c r="AC59" s="20"/>
+      <c r="AD59" s="20"/>
+      <c r="AE59" s="20"/>
+      <c r="AF59" s="20"/>
+      <c r="AG59" s="20"/>
+      <c r="AH59" s="20"/>
+    </row>
+    <row r="60" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4885,8 +5872,23 @@
         <v/>
       </c>
       <c r="S60" s="4"/>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T60" s="20"/>
+      <c r="U60" s="20"/>
+      <c r="V60" s="20"/>
+      <c r="W60" s="20"/>
+      <c r="X60" s="20"/>
+      <c r="Y60" s="20"/>
+      <c r="Z60" s="20"/>
+      <c r="AA60" s="20"/>
+      <c r="AB60" s="20"/>
+      <c r="AC60" s="20"/>
+      <c r="AD60" s="20"/>
+      <c r="AE60" s="20"/>
+      <c r="AF60" s="20"/>
+      <c r="AG60" s="20"/>
+      <c r="AH60" s="20"/>
+    </row>
+    <row r="61" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4927,8 +5929,23 @@
         <v/>
       </c>
       <c r="S61" s="4"/>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T61" s="20"/>
+      <c r="U61" s="20"/>
+      <c r="V61" s="20"/>
+      <c r="W61" s="20"/>
+      <c r="X61" s="20"/>
+      <c r="Y61" s="20"/>
+      <c r="Z61" s="20"/>
+      <c r="AA61" s="20"/>
+      <c r="AB61" s="20"/>
+      <c r="AC61" s="20"/>
+      <c r="AD61" s="20"/>
+      <c r="AE61" s="20"/>
+      <c r="AF61" s="20"/>
+      <c r="AG61" s="20"/>
+      <c r="AH61" s="20"/>
+    </row>
+    <row r="62" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4969,8 +5986,23 @@
         <v/>
       </c>
       <c r="S62" s="4"/>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T62" s="20"/>
+      <c r="U62" s="20"/>
+      <c r="V62" s="20"/>
+      <c r="W62" s="20"/>
+      <c r="X62" s="20"/>
+      <c r="Y62" s="20"/>
+      <c r="Z62" s="20"/>
+      <c r="AA62" s="20"/>
+      <c r="AB62" s="20"/>
+      <c r="AC62" s="20"/>
+      <c r="AD62" s="20"/>
+      <c r="AE62" s="20"/>
+      <c r="AF62" s="20"/>
+      <c r="AG62" s="20"/>
+      <c r="AH62" s="20"/>
+    </row>
+    <row r="63" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -5011,8 +6043,23 @@
         <v/>
       </c>
       <c r="S63" s="4"/>
-    </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T63" s="20"/>
+      <c r="U63" s="20"/>
+      <c r="V63" s="20"/>
+      <c r="W63" s="20"/>
+      <c r="X63" s="20"/>
+      <c r="Y63" s="20"/>
+      <c r="Z63" s="20"/>
+      <c r="AA63" s="20"/>
+      <c r="AB63" s="20"/>
+      <c r="AC63" s="20"/>
+      <c r="AD63" s="20"/>
+      <c r="AE63" s="20"/>
+      <c r="AF63" s="20"/>
+      <c r="AG63" s="20"/>
+      <c r="AH63" s="20"/>
+    </row>
+    <row r="64" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -5053,8 +6100,23 @@
         <v/>
       </c>
       <c r="S64" s="4"/>
-    </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T64" s="20"/>
+      <c r="U64" s="20"/>
+      <c r="V64" s="20"/>
+      <c r="W64" s="20"/>
+      <c r="X64" s="20"/>
+      <c r="Y64" s="20"/>
+      <c r="Z64" s="20"/>
+      <c r="AA64" s="20"/>
+      <c r="AB64" s="20"/>
+      <c r="AC64" s="20"/>
+      <c r="AD64" s="20"/>
+      <c r="AE64" s="20"/>
+      <c r="AF64" s="20"/>
+      <c r="AG64" s="20"/>
+      <c r="AH64" s="20"/>
+    </row>
+    <row r="65" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -5095,8 +6157,23 @@
         <v/>
       </c>
       <c r="S65" s="4"/>
-    </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T65" s="20"/>
+      <c r="U65" s="20"/>
+      <c r="V65" s="20"/>
+      <c r="W65" s="20"/>
+      <c r="X65" s="20"/>
+      <c r="Y65" s="20"/>
+      <c r="Z65" s="20"/>
+      <c r="AA65" s="20"/>
+      <c r="AB65" s="20"/>
+      <c r="AC65" s="20"/>
+      <c r="AD65" s="20"/>
+      <c r="AE65" s="20"/>
+      <c r="AF65" s="20"/>
+      <c r="AG65" s="20"/>
+      <c r="AH65" s="20"/>
+    </row>
+    <row r="66" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -5137,8 +6214,23 @@
         <v/>
       </c>
       <c r="S66" s="4"/>
-    </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T66" s="20"/>
+      <c r="U66" s="20"/>
+      <c r="V66" s="20"/>
+      <c r="W66" s="20"/>
+      <c r="X66" s="20"/>
+      <c r="Y66" s="20"/>
+      <c r="Z66" s="20"/>
+      <c r="AA66" s="20"/>
+      <c r="AB66" s="20"/>
+      <c r="AC66" s="20"/>
+      <c r="AD66" s="20"/>
+      <c r="AE66" s="20"/>
+      <c r="AF66" s="20"/>
+      <c r="AG66" s="20"/>
+      <c r="AH66" s="20"/>
+    </row>
+    <row r="67" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="str">
         <f t="shared" ref="A67:A130" si="10">IF(C67&lt;&gt;"",A66+1,"")</f>
         <v/>
@@ -5179,8 +6271,23 @@
         <v/>
       </c>
       <c r="S67" s="4"/>
-    </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T67" s="20"/>
+      <c r="U67" s="20"/>
+      <c r="V67" s="20"/>
+      <c r="W67" s="20"/>
+      <c r="X67" s="20"/>
+      <c r="Y67" s="20"/>
+      <c r="Z67" s="20"/>
+      <c r="AA67" s="20"/>
+      <c r="AB67" s="20"/>
+      <c r="AC67" s="20"/>
+      <c r="AD67" s="20"/>
+      <c r="AE67" s="20"/>
+      <c r="AF67" s="20"/>
+      <c r="AG67" s="20"/>
+      <c r="AH67" s="20"/>
+    </row>
+    <row r="68" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -5221,8 +6328,23 @@
         <v/>
       </c>
       <c r="S68" s="4"/>
-    </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T68" s="20"/>
+      <c r="U68" s="20"/>
+      <c r="V68" s="20"/>
+      <c r="W68" s="20"/>
+      <c r="X68" s="20"/>
+      <c r="Y68" s="20"/>
+      <c r="Z68" s="20"/>
+      <c r="AA68" s="20"/>
+      <c r="AB68" s="20"/>
+      <c r="AC68" s="20"/>
+      <c r="AD68" s="20"/>
+      <c r="AE68" s="20"/>
+      <c r="AF68" s="20"/>
+      <c r="AG68" s="20"/>
+      <c r="AH68" s="20"/>
+    </row>
+    <row r="69" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -5263,8 +6385,23 @@
         <v/>
       </c>
       <c r="S69" s="4"/>
-    </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T69" s="20"/>
+      <c r="U69" s="20"/>
+      <c r="V69" s="20"/>
+      <c r="W69" s="20"/>
+      <c r="X69" s="20"/>
+      <c r="Y69" s="20"/>
+      <c r="Z69" s="20"/>
+      <c r="AA69" s="20"/>
+      <c r="AB69" s="20"/>
+      <c r="AC69" s="20"/>
+      <c r="AD69" s="20"/>
+      <c r="AE69" s="20"/>
+      <c r="AF69" s="20"/>
+      <c r="AG69" s="20"/>
+      <c r="AH69" s="20"/>
+    </row>
+    <row r="70" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -5305,8 +6442,23 @@
         <v/>
       </c>
       <c r="S70" s="4"/>
-    </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T70" s="20"/>
+      <c r="U70" s="20"/>
+      <c r="V70" s="20"/>
+      <c r="W70" s="20"/>
+      <c r="X70" s="20"/>
+      <c r="Y70" s="20"/>
+      <c r="Z70" s="20"/>
+      <c r="AA70" s="20"/>
+      <c r="AB70" s="20"/>
+      <c r="AC70" s="20"/>
+      <c r="AD70" s="20"/>
+      <c r="AE70" s="20"/>
+      <c r="AF70" s="20"/>
+      <c r="AG70" s="20"/>
+      <c r="AH70" s="20"/>
+    </row>
+    <row r="71" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -5347,8 +6499,23 @@
         <v/>
       </c>
       <c r="S71" s="4"/>
-    </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T71" s="20"/>
+      <c r="U71" s="20"/>
+      <c r="V71" s="20"/>
+      <c r="W71" s="20"/>
+      <c r="X71" s="20"/>
+      <c r="Y71" s="20"/>
+      <c r="Z71" s="20"/>
+      <c r="AA71" s="20"/>
+      <c r="AB71" s="20"/>
+      <c r="AC71" s="20"/>
+      <c r="AD71" s="20"/>
+      <c r="AE71" s="20"/>
+      <c r="AF71" s="20"/>
+      <c r="AG71" s="20"/>
+      <c r="AH71" s="20"/>
+    </row>
+    <row r="72" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -5389,8 +6556,23 @@
         <v/>
       </c>
       <c r="S72" s="4"/>
-    </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T72" s="20"/>
+      <c r="U72" s="20"/>
+      <c r="V72" s="20"/>
+      <c r="W72" s="20"/>
+      <c r="X72" s="20"/>
+      <c r="Y72" s="20"/>
+      <c r="Z72" s="20"/>
+      <c r="AA72" s="20"/>
+      <c r="AB72" s="20"/>
+      <c r="AC72" s="20"/>
+      <c r="AD72" s="20"/>
+      <c r="AE72" s="20"/>
+      <c r="AF72" s="20"/>
+      <c r="AG72" s="20"/>
+      <c r="AH72" s="20"/>
+    </row>
+    <row r="73" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -5431,8 +6613,23 @@
         <v/>
       </c>
       <c r="S73" s="4"/>
-    </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T73" s="20"/>
+      <c r="U73" s="20"/>
+      <c r="V73" s="20"/>
+      <c r="W73" s="20"/>
+      <c r="X73" s="20"/>
+      <c r="Y73" s="20"/>
+      <c r="Z73" s="20"/>
+      <c r="AA73" s="20"/>
+      <c r="AB73" s="20"/>
+      <c r="AC73" s="20"/>
+      <c r="AD73" s="20"/>
+      <c r="AE73" s="20"/>
+      <c r="AF73" s="20"/>
+      <c r="AG73" s="20"/>
+      <c r="AH73" s="20"/>
+    </row>
+    <row r="74" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -5473,8 +6670,23 @@
         <v/>
       </c>
       <c r="S74" s="4"/>
-    </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T74" s="20"/>
+      <c r="U74" s="20"/>
+      <c r="V74" s="20"/>
+      <c r="W74" s="20"/>
+      <c r="X74" s="20"/>
+      <c r="Y74" s="20"/>
+      <c r="Z74" s="20"/>
+      <c r="AA74" s="20"/>
+      <c r="AB74" s="20"/>
+      <c r="AC74" s="20"/>
+      <c r="AD74" s="20"/>
+      <c r="AE74" s="20"/>
+      <c r="AF74" s="20"/>
+      <c r="AG74" s="20"/>
+      <c r="AH74" s="20"/>
+    </row>
+    <row r="75" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -5515,8 +6727,23 @@
         <v/>
       </c>
       <c r="S75" s="4"/>
-    </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T75" s="20"/>
+      <c r="U75" s="20"/>
+      <c r="V75" s="20"/>
+      <c r="W75" s="20"/>
+      <c r="X75" s="20"/>
+      <c r="Y75" s="20"/>
+      <c r="Z75" s="20"/>
+      <c r="AA75" s="20"/>
+      <c r="AB75" s="20"/>
+      <c r="AC75" s="20"/>
+      <c r="AD75" s="20"/>
+      <c r="AE75" s="20"/>
+      <c r="AF75" s="20"/>
+      <c r="AG75" s="20"/>
+      <c r="AH75" s="20"/>
+    </row>
+    <row r="76" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -5557,8 +6784,23 @@
         <v/>
       </c>
       <c r="S76" s="4"/>
-    </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T76" s="20"/>
+      <c r="U76" s="20"/>
+      <c r="V76" s="20"/>
+      <c r="W76" s="20"/>
+      <c r="X76" s="20"/>
+      <c r="Y76" s="20"/>
+      <c r="Z76" s="20"/>
+      <c r="AA76" s="20"/>
+      <c r="AB76" s="20"/>
+      <c r="AC76" s="20"/>
+      <c r="AD76" s="20"/>
+      <c r="AE76" s="20"/>
+      <c r="AF76" s="20"/>
+      <c r="AG76" s="20"/>
+      <c r="AH76" s="20"/>
+    </row>
+    <row r="77" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -5599,8 +6841,23 @@
         <v/>
       </c>
       <c r="S77" s="4"/>
-    </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T77" s="20"/>
+      <c r="U77" s="20"/>
+      <c r="V77" s="20"/>
+      <c r="W77" s="20"/>
+      <c r="X77" s="20"/>
+      <c r="Y77" s="20"/>
+      <c r="Z77" s="20"/>
+      <c r="AA77" s="20"/>
+      <c r="AB77" s="20"/>
+      <c r="AC77" s="20"/>
+      <c r="AD77" s="20"/>
+      <c r="AE77" s="20"/>
+      <c r="AF77" s="20"/>
+      <c r="AG77" s="20"/>
+      <c r="AH77" s="20"/>
+    </row>
+    <row r="78" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -5641,8 +6898,23 @@
         <v/>
       </c>
       <c r="S78" s="4"/>
-    </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T78" s="20"/>
+      <c r="U78" s="20"/>
+      <c r="V78" s="20"/>
+      <c r="W78" s="20"/>
+      <c r="X78" s="20"/>
+      <c r="Y78" s="20"/>
+      <c r="Z78" s="20"/>
+      <c r="AA78" s="20"/>
+      <c r="AB78" s="20"/>
+      <c r="AC78" s="20"/>
+      <c r="AD78" s="20"/>
+      <c r="AE78" s="20"/>
+      <c r="AF78" s="20"/>
+      <c r="AG78" s="20"/>
+      <c r="AH78" s="20"/>
+    </row>
+    <row r="79" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -5683,8 +6955,23 @@
         <v/>
       </c>
       <c r="S79" s="4"/>
-    </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T79" s="20"/>
+      <c r="U79" s="20"/>
+      <c r="V79" s="20"/>
+      <c r="W79" s="20"/>
+      <c r="X79" s="20"/>
+      <c r="Y79" s="20"/>
+      <c r="Z79" s="20"/>
+      <c r="AA79" s="20"/>
+      <c r="AB79" s="20"/>
+      <c r="AC79" s="20"/>
+      <c r="AD79" s="20"/>
+      <c r="AE79" s="20"/>
+      <c r="AF79" s="20"/>
+      <c r="AG79" s="20"/>
+      <c r="AH79" s="20"/>
+    </row>
+    <row r="80" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -5725,8 +7012,23 @@
         <v/>
       </c>
       <c r="S80" s="4"/>
-    </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T80" s="20"/>
+      <c r="U80" s="20"/>
+      <c r="V80" s="20"/>
+      <c r="W80" s="20"/>
+      <c r="X80" s="20"/>
+      <c r="Y80" s="20"/>
+      <c r="Z80" s="20"/>
+      <c r="AA80" s="20"/>
+      <c r="AB80" s="20"/>
+      <c r="AC80" s="20"/>
+      <c r="AD80" s="20"/>
+      <c r="AE80" s="20"/>
+      <c r="AF80" s="20"/>
+      <c r="AG80" s="20"/>
+      <c r="AH80" s="20"/>
+    </row>
+    <row r="81" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -5767,8 +7069,23 @@
         <v/>
       </c>
       <c r="S81" s="4"/>
-    </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T81" s="20"/>
+      <c r="U81" s="20"/>
+      <c r="V81" s="20"/>
+      <c r="W81" s="20"/>
+      <c r="X81" s="20"/>
+      <c r="Y81" s="20"/>
+      <c r="Z81" s="20"/>
+      <c r="AA81" s="20"/>
+      <c r="AB81" s="20"/>
+      <c r="AC81" s="20"/>
+      <c r="AD81" s="20"/>
+      <c r="AE81" s="20"/>
+      <c r="AF81" s="20"/>
+      <c r="AG81" s="20"/>
+      <c r="AH81" s="20"/>
+    </row>
+    <row r="82" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -5809,8 +7126,23 @@
         <v/>
       </c>
       <c r="S82" s="4"/>
-    </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T82" s="20"/>
+      <c r="U82" s="20"/>
+      <c r="V82" s="20"/>
+      <c r="W82" s="20"/>
+      <c r="X82" s="20"/>
+      <c r="Y82" s="20"/>
+      <c r="Z82" s="20"/>
+      <c r="AA82" s="20"/>
+      <c r="AB82" s="20"/>
+      <c r="AC82" s="20"/>
+      <c r="AD82" s="20"/>
+      <c r="AE82" s="20"/>
+      <c r="AF82" s="20"/>
+      <c r="AG82" s="20"/>
+      <c r="AH82" s="20"/>
+    </row>
+    <row r="83" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -5851,8 +7183,23 @@
         <v/>
       </c>
       <c r="S83" s="4"/>
-    </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T83" s="20"/>
+      <c r="U83" s="20"/>
+      <c r="V83" s="20"/>
+      <c r="W83" s="20"/>
+      <c r="X83" s="20"/>
+      <c r="Y83" s="20"/>
+      <c r="Z83" s="20"/>
+      <c r="AA83" s="20"/>
+      <c r="AB83" s="20"/>
+      <c r="AC83" s="20"/>
+      <c r="AD83" s="20"/>
+      <c r="AE83" s="20"/>
+      <c r="AF83" s="20"/>
+      <c r="AG83" s="20"/>
+      <c r="AH83" s="20"/>
+    </row>
+    <row r="84" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -5893,8 +7240,23 @@
         <v/>
       </c>
       <c r="S84" s="4"/>
-    </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T84" s="20"/>
+      <c r="U84" s="20"/>
+      <c r="V84" s="20"/>
+      <c r="W84" s="20"/>
+      <c r="X84" s="20"/>
+      <c r="Y84" s="20"/>
+      <c r="Z84" s="20"/>
+      <c r="AA84" s="20"/>
+      <c r="AB84" s="20"/>
+      <c r="AC84" s="20"/>
+      <c r="AD84" s="20"/>
+      <c r="AE84" s="20"/>
+      <c r="AF84" s="20"/>
+      <c r="AG84" s="20"/>
+      <c r="AH84" s="20"/>
+    </row>
+    <row r="85" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -5935,8 +7297,23 @@
         <v/>
       </c>
       <c r="S85" s="4"/>
-    </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T85" s="20"/>
+      <c r="U85" s="20"/>
+      <c r="V85" s="20"/>
+      <c r="W85" s="20"/>
+      <c r="X85" s="20"/>
+      <c r="Y85" s="20"/>
+      <c r="Z85" s="20"/>
+      <c r="AA85" s="20"/>
+      <c r="AB85" s="20"/>
+      <c r="AC85" s="20"/>
+      <c r="AD85" s="20"/>
+      <c r="AE85" s="20"/>
+      <c r="AF85" s="20"/>
+      <c r="AG85" s="20"/>
+      <c r="AH85" s="20"/>
+    </row>
+    <row r="86" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -5977,8 +7354,23 @@
         <v/>
       </c>
       <c r="S86" s="4"/>
-    </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T86" s="20"/>
+      <c r="U86" s="20"/>
+      <c r="V86" s="20"/>
+      <c r="W86" s="20"/>
+      <c r="X86" s="20"/>
+      <c r="Y86" s="20"/>
+      <c r="Z86" s="20"/>
+      <c r="AA86" s="20"/>
+      <c r="AB86" s="20"/>
+      <c r="AC86" s="20"/>
+      <c r="AD86" s="20"/>
+      <c r="AE86" s="20"/>
+      <c r="AF86" s="20"/>
+      <c r="AG86" s="20"/>
+      <c r="AH86" s="20"/>
+    </row>
+    <row r="87" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6019,8 +7411,23 @@
         <v/>
       </c>
       <c r="S87" s="4"/>
-    </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T87" s="20"/>
+      <c r="U87" s="20"/>
+      <c r="V87" s="20"/>
+      <c r="W87" s="20"/>
+      <c r="X87" s="20"/>
+      <c r="Y87" s="20"/>
+      <c r="Z87" s="20"/>
+      <c r="AA87" s="20"/>
+      <c r="AB87" s="20"/>
+      <c r="AC87" s="20"/>
+      <c r="AD87" s="20"/>
+      <c r="AE87" s="20"/>
+      <c r="AF87" s="20"/>
+      <c r="AG87" s="20"/>
+      <c r="AH87" s="20"/>
+    </row>
+    <row r="88" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6061,8 +7468,23 @@
         <v/>
       </c>
       <c r="S88" s="4"/>
-    </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T88" s="20"/>
+      <c r="U88" s="20"/>
+      <c r="V88" s="20"/>
+      <c r="W88" s="20"/>
+      <c r="X88" s="20"/>
+      <c r="Y88" s="20"/>
+      <c r="Z88" s="20"/>
+      <c r="AA88" s="20"/>
+      <c r="AB88" s="20"/>
+      <c r="AC88" s="20"/>
+      <c r="AD88" s="20"/>
+      <c r="AE88" s="20"/>
+      <c r="AF88" s="20"/>
+      <c r="AG88" s="20"/>
+      <c r="AH88" s="20"/>
+    </row>
+    <row r="89" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6103,8 +7525,23 @@
         <v/>
       </c>
       <c r="S89" s="4"/>
-    </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T89" s="20"/>
+      <c r="U89" s="20"/>
+      <c r="V89" s="20"/>
+      <c r="W89" s="20"/>
+      <c r="X89" s="20"/>
+      <c r="Y89" s="20"/>
+      <c r="Z89" s="20"/>
+      <c r="AA89" s="20"/>
+      <c r="AB89" s="20"/>
+      <c r="AC89" s="20"/>
+      <c r="AD89" s="20"/>
+      <c r="AE89" s="20"/>
+      <c r="AF89" s="20"/>
+      <c r="AG89" s="20"/>
+      <c r="AH89" s="20"/>
+    </row>
+    <row r="90" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6145,8 +7582,23 @@
         <v/>
       </c>
       <c r="S90" s="4"/>
-    </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T90" s="20"/>
+      <c r="U90" s="20"/>
+      <c r="V90" s="20"/>
+      <c r="W90" s="20"/>
+      <c r="X90" s="20"/>
+      <c r="Y90" s="20"/>
+      <c r="Z90" s="20"/>
+      <c r="AA90" s="20"/>
+      <c r="AB90" s="20"/>
+      <c r="AC90" s="20"/>
+      <c r="AD90" s="20"/>
+      <c r="AE90" s="20"/>
+      <c r="AF90" s="20"/>
+      <c r="AG90" s="20"/>
+      <c r="AH90" s="20"/>
+    </row>
+    <row r="91" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6187,8 +7639,23 @@
         <v/>
       </c>
       <c r="S91" s="4"/>
-    </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T91" s="20"/>
+      <c r="U91" s="20"/>
+      <c r="V91" s="20"/>
+      <c r="W91" s="20"/>
+      <c r="X91" s="20"/>
+      <c r="Y91" s="20"/>
+      <c r="Z91" s="20"/>
+      <c r="AA91" s="20"/>
+      <c r="AB91" s="20"/>
+      <c r="AC91" s="20"/>
+      <c r="AD91" s="20"/>
+      <c r="AE91" s="20"/>
+      <c r="AF91" s="20"/>
+      <c r="AG91" s="20"/>
+      <c r="AH91" s="20"/>
+    </row>
+    <row r="92" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6229,8 +7696,23 @@
         <v/>
       </c>
       <c r="S92" s="4"/>
-    </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T92" s="20"/>
+      <c r="U92" s="20"/>
+      <c r="V92" s="20"/>
+      <c r="W92" s="20"/>
+      <c r="X92" s="20"/>
+      <c r="Y92" s="20"/>
+      <c r="Z92" s="20"/>
+      <c r="AA92" s="20"/>
+      <c r="AB92" s="20"/>
+      <c r="AC92" s="20"/>
+      <c r="AD92" s="20"/>
+      <c r="AE92" s="20"/>
+      <c r="AF92" s="20"/>
+      <c r="AG92" s="20"/>
+      <c r="AH92" s="20"/>
+    </row>
+    <row r="93" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6271,8 +7753,23 @@
         <v/>
       </c>
       <c r="S93" s="4"/>
-    </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T93" s="20"/>
+      <c r="U93" s="20"/>
+      <c r="V93" s="20"/>
+      <c r="W93" s="20"/>
+      <c r="X93" s="20"/>
+      <c r="Y93" s="20"/>
+      <c r="Z93" s="20"/>
+      <c r="AA93" s="20"/>
+      <c r="AB93" s="20"/>
+      <c r="AC93" s="20"/>
+      <c r="AD93" s="20"/>
+      <c r="AE93" s="20"/>
+      <c r="AF93" s="20"/>
+      <c r="AG93" s="20"/>
+      <c r="AH93" s="20"/>
+    </row>
+    <row r="94" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6313,8 +7810,23 @@
         <v/>
       </c>
       <c r="S94" s="4"/>
-    </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T94" s="20"/>
+      <c r="U94" s="20"/>
+      <c r="V94" s="20"/>
+      <c r="W94" s="20"/>
+      <c r="X94" s="20"/>
+      <c r="Y94" s="20"/>
+      <c r="Z94" s="20"/>
+      <c r="AA94" s="20"/>
+      <c r="AB94" s="20"/>
+      <c r="AC94" s="20"/>
+      <c r="AD94" s="20"/>
+      <c r="AE94" s="20"/>
+      <c r="AF94" s="20"/>
+      <c r="AG94" s="20"/>
+      <c r="AH94" s="20"/>
+    </row>
+    <row r="95" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6355,8 +7867,23 @@
         <v/>
       </c>
       <c r="S95" s="4"/>
-    </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T95" s="20"/>
+      <c r="U95" s="20"/>
+      <c r="V95" s="20"/>
+      <c r="W95" s="20"/>
+      <c r="X95" s="20"/>
+      <c r="Y95" s="20"/>
+      <c r="Z95" s="20"/>
+      <c r="AA95" s="20"/>
+      <c r="AB95" s="20"/>
+      <c r="AC95" s="20"/>
+      <c r="AD95" s="20"/>
+      <c r="AE95" s="20"/>
+      <c r="AF95" s="20"/>
+      <c r="AG95" s="20"/>
+      <c r="AH95" s="20"/>
+    </row>
+    <row r="96" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6397,8 +7924,23 @@
         <v/>
       </c>
       <c r="S96" s="4"/>
-    </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T96" s="20"/>
+      <c r="U96" s="20"/>
+      <c r="V96" s="20"/>
+      <c r="W96" s="20"/>
+      <c r="X96" s="20"/>
+      <c r="Y96" s="20"/>
+      <c r="Z96" s="20"/>
+      <c r="AA96" s="20"/>
+      <c r="AB96" s="20"/>
+      <c r="AC96" s="20"/>
+      <c r="AD96" s="20"/>
+      <c r="AE96" s="20"/>
+      <c r="AF96" s="20"/>
+      <c r="AG96" s="20"/>
+      <c r="AH96" s="20"/>
+    </row>
+    <row r="97" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6439,8 +7981,23 @@
         <v/>
       </c>
       <c r="S97" s="4"/>
-    </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T97" s="20"/>
+      <c r="U97" s="20"/>
+      <c r="V97" s="20"/>
+      <c r="W97" s="20"/>
+      <c r="X97" s="20"/>
+      <c r="Y97" s="20"/>
+      <c r="Z97" s="20"/>
+      <c r="AA97" s="20"/>
+      <c r="AB97" s="20"/>
+      <c r="AC97" s="20"/>
+      <c r="AD97" s="20"/>
+      <c r="AE97" s="20"/>
+      <c r="AF97" s="20"/>
+      <c r="AG97" s="20"/>
+      <c r="AH97" s="20"/>
+    </row>
+    <row r="98" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6481,8 +8038,23 @@
         <v/>
       </c>
       <c r="S98" s="4"/>
-    </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T98" s="20"/>
+      <c r="U98" s="20"/>
+      <c r="V98" s="20"/>
+      <c r="W98" s="20"/>
+      <c r="X98" s="20"/>
+      <c r="Y98" s="20"/>
+      <c r="Z98" s="20"/>
+      <c r="AA98" s="20"/>
+      <c r="AB98" s="20"/>
+      <c r="AC98" s="20"/>
+      <c r="AD98" s="20"/>
+      <c r="AE98" s="20"/>
+      <c r="AF98" s="20"/>
+      <c r="AG98" s="20"/>
+      <c r="AH98" s="20"/>
+    </row>
+    <row r="99" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6523,8 +8095,23 @@
         <v/>
       </c>
       <c r="S99" s="4"/>
-    </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T99" s="20"/>
+      <c r="U99" s="20"/>
+      <c r="V99" s="20"/>
+      <c r="W99" s="20"/>
+      <c r="X99" s="20"/>
+      <c r="Y99" s="20"/>
+      <c r="Z99" s="20"/>
+      <c r="AA99" s="20"/>
+      <c r="AB99" s="20"/>
+      <c r="AC99" s="20"/>
+      <c r="AD99" s="20"/>
+      <c r="AE99" s="20"/>
+      <c r="AF99" s="20"/>
+      <c r="AG99" s="20"/>
+      <c r="AH99" s="20"/>
+    </row>
+    <row r="100" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6565,8 +8152,23 @@
         <v/>
       </c>
       <c r="S100" s="4"/>
-    </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T100" s="20"/>
+      <c r="U100" s="20"/>
+      <c r="V100" s="20"/>
+      <c r="W100" s="20"/>
+      <c r="X100" s="20"/>
+      <c r="Y100" s="20"/>
+      <c r="Z100" s="20"/>
+      <c r="AA100" s="20"/>
+      <c r="AB100" s="20"/>
+      <c r="AC100" s="20"/>
+      <c r="AD100" s="20"/>
+      <c r="AE100" s="20"/>
+      <c r="AF100" s="20"/>
+      <c r="AG100" s="20"/>
+      <c r="AH100" s="20"/>
+    </row>
+    <row r="101" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6607,8 +8209,23 @@
         <v/>
       </c>
       <c r="S101" s="4"/>
-    </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T101" s="20"/>
+      <c r="U101" s="20"/>
+      <c r="V101" s="20"/>
+      <c r="W101" s="20"/>
+      <c r="X101" s="20"/>
+      <c r="Y101" s="20"/>
+      <c r="Z101" s="20"/>
+      <c r="AA101" s="20"/>
+      <c r="AB101" s="20"/>
+      <c r="AC101" s="20"/>
+      <c r="AD101" s="20"/>
+      <c r="AE101" s="20"/>
+      <c r="AF101" s="20"/>
+      <c r="AG101" s="20"/>
+      <c r="AH101" s="20"/>
+    </row>
+    <row r="102" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6649,8 +8266,23 @@
         <v/>
       </c>
       <c r="S102" s="4"/>
-    </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T102" s="20"/>
+      <c r="U102" s="20"/>
+      <c r="V102" s="20"/>
+      <c r="W102" s="20"/>
+      <c r="X102" s="20"/>
+      <c r="Y102" s="20"/>
+      <c r="Z102" s="20"/>
+      <c r="AA102" s="20"/>
+      <c r="AB102" s="20"/>
+      <c r="AC102" s="20"/>
+      <c r="AD102" s="20"/>
+      <c r="AE102" s="20"/>
+      <c r="AF102" s="20"/>
+      <c r="AG102" s="20"/>
+      <c r="AH102" s="20"/>
+    </row>
+    <row r="103" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6691,8 +8323,23 @@
         <v/>
       </c>
       <c r="S103" s="4"/>
-    </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T103" s="20"/>
+      <c r="U103" s="20"/>
+      <c r="V103" s="20"/>
+      <c r="W103" s="20"/>
+      <c r="X103" s="20"/>
+      <c r="Y103" s="20"/>
+      <c r="Z103" s="20"/>
+      <c r="AA103" s="20"/>
+      <c r="AB103" s="20"/>
+      <c r="AC103" s="20"/>
+      <c r="AD103" s="20"/>
+      <c r="AE103" s="20"/>
+      <c r="AF103" s="20"/>
+      <c r="AG103" s="20"/>
+      <c r="AH103" s="20"/>
+    </row>
+    <row r="104" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6733,8 +8380,23 @@
         <v/>
       </c>
       <c r="S104" s="4"/>
-    </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T104" s="20"/>
+      <c r="U104" s="20"/>
+      <c r="V104" s="20"/>
+      <c r="W104" s="20"/>
+      <c r="X104" s="20"/>
+      <c r="Y104" s="20"/>
+      <c r="Z104" s="20"/>
+      <c r="AA104" s="20"/>
+      <c r="AB104" s="20"/>
+      <c r="AC104" s="20"/>
+      <c r="AD104" s="20"/>
+      <c r="AE104" s="20"/>
+      <c r="AF104" s="20"/>
+      <c r="AG104" s="20"/>
+      <c r="AH104" s="20"/>
+    </row>
+    <row r="105" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6775,8 +8437,23 @@
         <v/>
       </c>
       <c r="S105" s="4"/>
-    </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T105" s="20"/>
+      <c r="U105" s="20"/>
+      <c r="V105" s="20"/>
+      <c r="W105" s="20"/>
+      <c r="X105" s="20"/>
+      <c r="Y105" s="20"/>
+      <c r="Z105" s="20"/>
+      <c r="AA105" s="20"/>
+      <c r="AB105" s="20"/>
+      <c r="AC105" s="20"/>
+      <c r="AD105" s="20"/>
+      <c r="AE105" s="20"/>
+      <c r="AF105" s="20"/>
+      <c r="AG105" s="20"/>
+      <c r="AH105" s="20"/>
+    </row>
+    <row r="106" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6817,8 +8494,23 @@
         <v/>
       </c>
       <c r="S106" s="4"/>
-    </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T106" s="20"/>
+      <c r="U106" s="20"/>
+      <c r="V106" s="20"/>
+      <c r="W106" s="20"/>
+      <c r="X106" s="20"/>
+      <c r="Y106" s="20"/>
+      <c r="Z106" s="20"/>
+      <c r="AA106" s="20"/>
+      <c r="AB106" s="20"/>
+      <c r="AC106" s="20"/>
+      <c r="AD106" s="20"/>
+      <c r="AE106" s="20"/>
+      <c r="AF106" s="20"/>
+      <c r="AG106" s="20"/>
+      <c r="AH106" s="20"/>
+    </row>
+    <row r="107" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6859,8 +8551,23 @@
         <v/>
       </c>
       <c r="S107" s="4"/>
-    </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T107" s="20"/>
+      <c r="U107" s="20"/>
+      <c r="V107" s="20"/>
+      <c r="W107" s="20"/>
+      <c r="X107" s="20"/>
+      <c r="Y107" s="20"/>
+      <c r="Z107" s="20"/>
+      <c r="AA107" s="20"/>
+      <c r="AB107" s="20"/>
+      <c r="AC107" s="20"/>
+      <c r="AD107" s="20"/>
+      <c r="AE107" s="20"/>
+      <c r="AF107" s="20"/>
+      <c r="AG107" s="20"/>
+      <c r="AH107" s="20"/>
+    </row>
+    <row r="108" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6901,8 +8608,23 @@
         <v/>
       </c>
       <c r="S108" s="4"/>
-    </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T108" s="20"/>
+      <c r="U108" s="20"/>
+      <c r="V108" s="20"/>
+      <c r="W108" s="20"/>
+      <c r="X108" s="20"/>
+      <c r="Y108" s="20"/>
+      <c r="Z108" s="20"/>
+      <c r="AA108" s="20"/>
+      <c r="AB108" s="20"/>
+      <c r="AC108" s="20"/>
+      <c r="AD108" s="20"/>
+      <c r="AE108" s="20"/>
+      <c r="AF108" s="20"/>
+      <c r="AG108" s="20"/>
+      <c r="AH108" s="20"/>
+    </row>
+    <row r="109" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6943,8 +8665,23 @@
         <v/>
       </c>
       <c r="S109" s="4"/>
-    </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T109" s="20"/>
+      <c r="U109" s="20"/>
+      <c r="V109" s="20"/>
+      <c r="W109" s="20"/>
+      <c r="X109" s="20"/>
+      <c r="Y109" s="20"/>
+      <c r="Z109" s="20"/>
+      <c r="AA109" s="20"/>
+      <c r="AB109" s="20"/>
+      <c r="AC109" s="20"/>
+      <c r="AD109" s="20"/>
+      <c r="AE109" s="20"/>
+      <c r="AF109" s="20"/>
+      <c r="AG109" s="20"/>
+      <c r="AH109" s="20"/>
+    </row>
+    <row r="110" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -6985,8 +8722,23 @@
         <v/>
       </c>
       <c r="S110" s="4"/>
-    </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T110" s="20"/>
+      <c r="U110" s="20"/>
+      <c r="V110" s="20"/>
+      <c r="W110" s="20"/>
+      <c r="X110" s="20"/>
+      <c r="Y110" s="20"/>
+      <c r="Z110" s="20"/>
+      <c r="AA110" s="20"/>
+      <c r="AB110" s="20"/>
+      <c r="AC110" s="20"/>
+      <c r="AD110" s="20"/>
+      <c r="AE110" s="20"/>
+      <c r="AF110" s="20"/>
+      <c r="AG110" s="20"/>
+      <c r="AH110" s="20"/>
+    </row>
+    <row r="111" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -7027,8 +8779,23 @@
         <v/>
       </c>
       <c r="S111" s="4"/>
-    </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T111" s="20"/>
+      <c r="U111" s="20"/>
+      <c r="V111" s="20"/>
+      <c r="W111" s="20"/>
+      <c r="X111" s="20"/>
+      <c r="Y111" s="20"/>
+      <c r="Z111" s="20"/>
+      <c r="AA111" s="20"/>
+      <c r="AB111" s="20"/>
+      <c r="AC111" s="20"/>
+      <c r="AD111" s="20"/>
+      <c r="AE111" s="20"/>
+      <c r="AF111" s="20"/>
+      <c r="AG111" s="20"/>
+      <c r="AH111" s="20"/>
+    </row>
+    <row r="112" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -7069,8 +8836,23 @@
         <v/>
       </c>
       <c r="S112" s="4"/>
-    </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T112" s="20"/>
+      <c r="U112" s="20"/>
+      <c r="V112" s="20"/>
+      <c r="W112" s="20"/>
+      <c r="X112" s="20"/>
+      <c r="Y112" s="20"/>
+      <c r="Z112" s="20"/>
+      <c r="AA112" s="20"/>
+      <c r="AB112" s="20"/>
+      <c r="AC112" s="20"/>
+      <c r="AD112" s="20"/>
+      <c r="AE112" s="20"/>
+      <c r="AF112" s="20"/>
+      <c r="AG112" s="20"/>
+      <c r="AH112" s="20"/>
+    </row>
+    <row r="113" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -7111,8 +8893,23 @@
         <v/>
       </c>
       <c r="S113" s="4"/>
-    </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T113" s="20"/>
+      <c r="U113" s="20"/>
+      <c r="V113" s="20"/>
+      <c r="W113" s="20"/>
+      <c r="X113" s="20"/>
+      <c r="Y113" s="20"/>
+      <c r="Z113" s="20"/>
+      <c r="AA113" s="20"/>
+      <c r="AB113" s="20"/>
+      <c r="AC113" s="20"/>
+      <c r="AD113" s="20"/>
+      <c r="AE113" s="20"/>
+      <c r="AF113" s="20"/>
+      <c r="AG113" s="20"/>
+      <c r="AH113" s="20"/>
+    </row>
+    <row r="114" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -7153,8 +8950,23 @@
         <v/>
       </c>
       <c r="S114" s="4"/>
-    </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T114" s="20"/>
+      <c r="U114" s="20"/>
+      <c r="V114" s="20"/>
+      <c r="W114" s="20"/>
+      <c r="X114" s="20"/>
+      <c r="Y114" s="20"/>
+      <c r="Z114" s="20"/>
+      <c r="AA114" s="20"/>
+      <c r="AB114" s="20"/>
+      <c r="AC114" s="20"/>
+      <c r="AD114" s="20"/>
+      <c r="AE114" s="20"/>
+      <c r="AF114" s="20"/>
+      <c r="AG114" s="20"/>
+      <c r="AH114" s="20"/>
+    </row>
+    <row r="115" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -7195,8 +9007,23 @@
         <v/>
       </c>
       <c r="S115" s="4"/>
-    </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T115" s="20"/>
+      <c r="U115" s="20"/>
+      <c r="V115" s="20"/>
+      <c r="W115" s="20"/>
+      <c r="X115" s="20"/>
+      <c r="Y115" s="20"/>
+      <c r="Z115" s="20"/>
+      <c r="AA115" s="20"/>
+      <c r="AB115" s="20"/>
+      <c r="AC115" s="20"/>
+      <c r="AD115" s="20"/>
+      <c r="AE115" s="20"/>
+      <c r="AF115" s="20"/>
+      <c r="AG115" s="20"/>
+      <c r="AH115" s="20"/>
+    </row>
+    <row r="116" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -7237,8 +9064,23 @@
         <v/>
       </c>
       <c r="S116" s="4"/>
-    </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T116" s="20"/>
+      <c r="U116" s="20"/>
+      <c r="V116" s="20"/>
+      <c r="W116" s="20"/>
+      <c r="X116" s="20"/>
+      <c r="Y116" s="20"/>
+      <c r="Z116" s="20"/>
+      <c r="AA116" s="20"/>
+      <c r="AB116" s="20"/>
+      <c r="AC116" s="20"/>
+      <c r="AD116" s="20"/>
+      <c r="AE116" s="20"/>
+      <c r="AF116" s="20"/>
+      <c r="AG116" s="20"/>
+      <c r="AH116" s="20"/>
+    </row>
+    <row r="117" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -7279,8 +9121,23 @@
         <v/>
       </c>
       <c r="S117" s="4"/>
-    </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T117" s="20"/>
+      <c r="U117" s="20"/>
+      <c r="V117" s="20"/>
+      <c r="W117" s="20"/>
+      <c r="X117" s="20"/>
+      <c r="Y117" s="20"/>
+      <c r="Z117" s="20"/>
+      <c r="AA117" s="20"/>
+      <c r="AB117" s="20"/>
+      <c r="AC117" s="20"/>
+      <c r="AD117" s="20"/>
+      <c r="AE117" s="20"/>
+      <c r="AF117" s="20"/>
+      <c r="AG117" s="20"/>
+      <c r="AH117" s="20"/>
+    </row>
+    <row r="118" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -7321,8 +9178,23 @@
         <v/>
       </c>
       <c r="S118" s="4"/>
-    </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T118" s="20"/>
+      <c r="U118" s="20"/>
+      <c r="V118" s="20"/>
+      <c r="W118" s="20"/>
+      <c r="X118" s="20"/>
+      <c r="Y118" s="20"/>
+      <c r="Z118" s="20"/>
+      <c r="AA118" s="20"/>
+      <c r="AB118" s="20"/>
+      <c r="AC118" s="20"/>
+      <c r="AD118" s="20"/>
+      <c r="AE118" s="20"/>
+      <c r="AF118" s="20"/>
+      <c r="AG118" s="20"/>
+      <c r="AH118" s="20"/>
+    </row>
+    <row r="119" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -7363,8 +9235,23 @@
         <v/>
       </c>
       <c r="S119" s="4"/>
-    </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T119" s="20"/>
+      <c r="U119" s="20"/>
+      <c r="V119" s="20"/>
+      <c r="W119" s="20"/>
+      <c r="X119" s="20"/>
+      <c r="Y119" s="20"/>
+      <c r="Z119" s="20"/>
+      <c r="AA119" s="20"/>
+      <c r="AB119" s="20"/>
+      <c r="AC119" s="20"/>
+      <c r="AD119" s="20"/>
+      <c r="AE119" s="20"/>
+      <c r="AF119" s="20"/>
+      <c r="AG119" s="20"/>
+      <c r="AH119" s="20"/>
+    </row>
+    <row r="120" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -7405,8 +9292,23 @@
         <v/>
       </c>
       <c r="S120" s="4"/>
-    </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T120" s="20"/>
+      <c r="U120" s="20"/>
+      <c r="V120" s="20"/>
+      <c r="W120" s="20"/>
+      <c r="X120" s="20"/>
+      <c r="Y120" s="20"/>
+      <c r="Z120" s="20"/>
+      <c r="AA120" s="20"/>
+      <c r="AB120" s="20"/>
+      <c r="AC120" s="20"/>
+      <c r="AD120" s="20"/>
+      <c r="AE120" s="20"/>
+      <c r="AF120" s="20"/>
+      <c r="AG120" s="20"/>
+      <c r="AH120" s="20"/>
+    </row>
+    <row r="121" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -7447,8 +9349,23 @@
         <v/>
       </c>
       <c r="S121" s="4"/>
-    </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T121" s="20"/>
+      <c r="U121" s="20"/>
+      <c r="V121" s="20"/>
+      <c r="W121" s="20"/>
+      <c r="X121" s="20"/>
+      <c r="Y121" s="20"/>
+      <c r="Z121" s="20"/>
+      <c r="AA121" s="20"/>
+      <c r="AB121" s="20"/>
+      <c r="AC121" s="20"/>
+      <c r="AD121" s="20"/>
+      <c r="AE121" s="20"/>
+      <c r="AF121" s="20"/>
+      <c r="AG121" s="20"/>
+      <c r="AH121" s="20"/>
+    </row>
+    <row r="122" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -7489,8 +9406,23 @@
         <v/>
       </c>
       <c r="S122" s="4"/>
-    </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T122" s="20"/>
+      <c r="U122" s="20"/>
+      <c r="V122" s="20"/>
+      <c r="W122" s="20"/>
+      <c r="X122" s="20"/>
+      <c r="Y122" s="20"/>
+      <c r="Z122" s="20"/>
+      <c r="AA122" s="20"/>
+      <c r="AB122" s="20"/>
+      <c r="AC122" s="20"/>
+      <c r="AD122" s="20"/>
+      <c r="AE122" s="20"/>
+      <c r="AF122" s="20"/>
+      <c r="AG122" s="20"/>
+      <c r="AH122" s="20"/>
+    </row>
+    <row r="123" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -7531,8 +9463,23 @@
         <v/>
       </c>
       <c r="S123" s="4"/>
-    </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T123" s="20"/>
+      <c r="U123" s="20"/>
+      <c r="V123" s="20"/>
+      <c r="W123" s="20"/>
+      <c r="X123" s="20"/>
+      <c r="Y123" s="20"/>
+      <c r="Z123" s="20"/>
+      <c r="AA123" s="20"/>
+      <c r="AB123" s="20"/>
+      <c r="AC123" s="20"/>
+      <c r="AD123" s="20"/>
+      <c r="AE123" s="20"/>
+      <c r="AF123" s="20"/>
+      <c r="AG123" s="20"/>
+      <c r="AH123" s="20"/>
+    </row>
+    <row r="124" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -7573,8 +9520,23 @@
         <v/>
       </c>
       <c r="S124" s="4"/>
-    </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T124" s="20"/>
+      <c r="U124" s="20"/>
+      <c r="V124" s="20"/>
+      <c r="W124" s="20"/>
+      <c r="X124" s="20"/>
+      <c r="Y124" s="20"/>
+      <c r="Z124" s="20"/>
+      <c r="AA124" s="20"/>
+      <c r="AB124" s="20"/>
+      <c r="AC124" s="20"/>
+      <c r="AD124" s="20"/>
+      <c r="AE124" s="20"/>
+      <c r="AF124" s="20"/>
+      <c r="AG124" s="20"/>
+      <c r="AH124" s="20"/>
+    </row>
+    <row r="125" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -7615,8 +9577,23 @@
         <v/>
       </c>
       <c r="S125" s="4"/>
-    </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T125" s="20"/>
+      <c r="U125" s="20"/>
+      <c r="V125" s="20"/>
+      <c r="W125" s="20"/>
+      <c r="X125" s="20"/>
+      <c r="Y125" s="20"/>
+      <c r="Z125" s="20"/>
+      <c r="AA125" s="20"/>
+      <c r="AB125" s="20"/>
+      <c r="AC125" s="20"/>
+      <c r="AD125" s="20"/>
+      <c r="AE125" s="20"/>
+      <c r="AF125" s="20"/>
+      <c r="AG125" s="20"/>
+      <c r="AH125" s="20"/>
+    </row>
+    <row r="126" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -7657,8 +9634,23 @@
         <v/>
       </c>
       <c r="S126" s="4"/>
-    </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T126" s="20"/>
+      <c r="U126" s="20"/>
+      <c r="V126" s="20"/>
+      <c r="W126" s="20"/>
+      <c r="X126" s="20"/>
+      <c r="Y126" s="20"/>
+      <c r="Z126" s="20"/>
+      <c r="AA126" s="20"/>
+      <c r="AB126" s="20"/>
+      <c r="AC126" s="20"/>
+      <c r="AD126" s="20"/>
+      <c r="AE126" s="20"/>
+      <c r="AF126" s="20"/>
+      <c r="AG126" s="20"/>
+      <c r="AH126" s="20"/>
+    </row>
+    <row r="127" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -7699,8 +9691,23 @@
         <v/>
       </c>
       <c r="S127" s="4"/>
-    </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T127" s="20"/>
+      <c r="U127" s="20"/>
+      <c r="V127" s="20"/>
+      <c r="W127" s="20"/>
+      <c r="X127" s="20"/>
+      <c r="Y127" s="20"/>
+      <c r="Z127" s="20"/>
+      <c r="AA127" s="20"/>
+      <c r="AB127" s="20"/>
+      <c r="AC127" s="20"/>
+      <c r="AD127" s="20"/>
+      <c r="AE127" s="20"/>
+      <c r="AF127" s="20"/>
+      <c r="AG127" s="20"/>
+      <c r="AH127" s="20"/>
+    </row>
+    <row r="128" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -7741,8 +9748,23 @@
         <v/>
       </c>
       <c r="S128" s="4"/>
-    </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T128" s="20"/>
+      <c r="U128" s="20"/>
+      <c r="V128" s="20"/>
+      <c r="W128" s="20"/>
+      <c r="X128" s="20"/>
+      <c r="Y128" s="20"/>
+      <c r="Z128" s="20"/>
+      <c r="AA128" s="20"/>
+      <c r="AB128" s="20"/>
+      <c r="AC128" s="20"/>
+      <c r="AD128" s="20"/>
+      <c r="AE128" s="20"/>
+      <c r="AF128" s="20"/>
+      <c r="AG128" s="20"/>
+      <c r="AH128" s="20"/>
+    </row>
+    <row r="129" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -7783,8 +9805,23 @@
         <v/>
       </c>
       <c r="S129" s="4"/>
-    </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T129" s="20"/>
+      <c r="U129" s="20"/>
+      <c r="V129" s="20"/>
+      <c r="W129" s="20"/>
+      <c r="X129" s="20"/>
+      <c r="Y129" s="20"/>
+      <c r="Z129" s="20"/>
+      <c r="AA129" s="20"/>
+      <c r="AB129" s="20"/>
+      <c r="AC129" s="20"/>
+      <c r="AD129" s="20"/>
+      <c r="AE129" s="20"/>
+      <c r="AF129" s="20"/>
+      <c r="AG129" s="20"/>
+      <c r="AH129" s="20"/>
+    </row>
+    <row r="130" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -7825,8 +9862,23 @@
         <v/>
       </c>
       <c r="S130" s="4"/>
-    </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T130" s="20"/>
+      <c r="U130" s="20"/>
+      <c r="V130" s="20"/>
+      <c r="W130" s="20"/>
+      <c r="X130" s="20"/>
+      <c r="Y130" s="20"/>
+      <c r="Z130" s="20"/>
+      <c r="AA130" s="20"/>
+      <c r="AB130" s="20"/>
+      <c r="AC130" s="20"/>
+      <c r="AD130" s="20"/>
+      <c r="AE130" s="20"/>
+      <c r="AF130" s="20"/>
+      <c r="AG130" s="20"/>
+      <c r="AH130" s="20"/>
+    </row>
+    <row r="131" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="str">
         <f t="shared" ref="A131:A168" si="14">IF(C131&lt;&gt;"",A130+1,"")</f>
         <v/>
@@ -7867,8 +9919,23 @@
         <v/>
       </c>
       <c r="S131" s="4"/>
-    </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T131" s="20"/>
+      <c r="U131" s="20"/>
+      <c r="V131" s="20"/>
+      <c r="W131" s="20"/>
+      <c r="X131" s="20"/>
+      <c r="Y131" s="20"/>
+      <c r="Z131" s="20"/>
+      <c r="AA131" s="20"/>
+      <c r="AB131" s="20"/>
+      <c r="AC131" s="20"/>
+      <c r="AD131" s="20"/>
+      <c r="AE131" s="20"/>
+      <c r="AF131" s="20"/>
+      <c r="AG131" s="20"/>
+      <c r="AH131" s="20"/>
+    </row>
+    <row r="132" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -7909,8 +9976,23 @@
         <v/>
       </c>
       <c r="S132" s="4"/>
-    </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T132" s="20"/>
+      <c r="U132" s="20"/>
+      <c r="V132" s="20"/>
+      <c r="W132" s="20"/>
+      <c r="X132" s="20"/>
+      <c r="Y132" s="20"/>
+      <c r="Z132" s="20"/>
+      <c r="AA132" s="20"/>
+      <c r="AB132" s="20"/>
+      <c r="AC132" s="20"/>
+      <c r="AD132" s="20"/>
+      <c r="AE132" s="20"/>
+      <c r="AF132" s="20"/>
+      <c r="AG132" s="20"/>
+      <c r="AH132" s="20"/>
+    </row>
+    <row r="133" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -7951,8 +10033,23 @@
         <v/>
       </c>
       <c r="S133" s="4"/>
-    </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T133" s="20"/>
+      <c r="U133" s="20"/>
+      <c r="V133" s="20"/>
+      <c r="W133" s="20"/>
+      <c r="X133" s="20"/>
+      <c r="Y133" s="20"/>
+      <c r="Z133" s="20"/>
+      <c r="AA133" s="20"/>
+      <c r="AB133" s="20"/>
+      <c r="AC133" s="20"/>
+      <c r="AD133" s="20"/>
+      <c r="AE133" s="20"/>
+      <c r="AF133" s="20"/>
+      <c r="AG133" s="20"/>
+      <c r="AH133" s="20"/>
+    </row>
+    <row r="134" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -7993,8 +10090,23 @@
         <v/>
       </c>
       <c r="S134" s="4"/>
-    </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T134" s="20"/>
+      <c r="U134" s="20"/>
+      <c r="V134" s="20"/>
+      <c r="W134" s="20"/>
+      <c r="X134" s="20"/>
+      <c r="Y134" s="20"/>
+      <c r="Z134" s="20"/>
+      <c r="AA134" s="20"/>
+      <c r="AB134" s="20"/>
+      <c r="AC134" s="20"/>
+      <c r="AD134" s="20"/>
+      <c r="AE134" s="20"/>
+      <c r="AF134" s="20"/>
+      <c r="AG134" s="20"/>
+      <c r="AH134" s="20"/>
+    </row>
+    <row r="135" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -8035,8 +10147,23 @@
         <v/>
       </c>
       <c r="S135" s="4"/>
-    </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T135" s="20"/>
+      <c r="U135" s="20"/>
+      <c r="V135" s="20"/>
+      <c r="W135" s="20"/>
+      <c r="X135" s="20"/>
+      <c r="Y135" s="20"/>
+      <c r="Z135" s="20"/>
+      <c r="AA135" s="20"/>
+      <c r="AB135" s="20"/>
+      <c r="AC135" s="20"/>
+      <c r="AD135" s="20"/>
+      <c r="AE135" s="20"/>
+      <c r="AF135" s="20"/>
+      <c r="AG135" s="20"/>
+      <c r="AH135" s="20"/>
+    </row>
+    <row r="136" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -8077,8 +10204,23 @@
         <v/>
       </c>
       <c r="S136" s="4"/>
-    </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T136" s="20"/>
+      <c r="U136" s="20"/>
+      <c r="V136" s="20"/>
+      <c r="W136" s="20"/>
+      <c r="X136" s="20"/>
+      <c r="Y136" s="20"/>
+      <c r="Z136" s="20"/>
+      <c r="AA136" s="20"/>
+      <c r="AB136" s="20"/>
+      <c r="AC136" s="20"/>
+      <c r="AD136" s="20"/>
+      <c r="AE136" s="20"/>
+      <c r="AF136" s="20"/>
+      <c r="AG136" s="20"/>
+      <c r="AH136" s="20"/>
+    </row>
+    <row r="137" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -8119,8 +10261,23 @@
         <v/>
       </c>
       <c r="S137" s="4"/>
-    </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T137" s="20"/>
+      <c r="U137" s="20"/>
+      <c r="V137" s="20"/>
+      <c r="W137" s="20"/>
+      <c r="X137" s="20"/>
+      <c r="Y137" s="20"/>
+      <c r="Z137" s="20"/>
+      <c r="AA137" s="20"/>
+      <c r="AB137" s="20"/>
+      <c r="AC137" s="20"/>
+      <c r="AD137" s="20"/>
+      <c r="AE137" s="20"/>
+      <c r="AF137" s="20"/>
+      <c r="AG137" s="20"/>
+      <c r="AH137" s="20"/>
+    </row>
+    <row r="138" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -8161,8 +10318,23 @@
         <v/>
       </c>
       <c r="S138" s="4"/>
-    </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T138" s="20"/>
+      <c r="U138" s="20"/>
+      <c r="V138" s="20"/>
+      <c r="W138" s="20"/>
+      <c r="X138" s="20"/>
+      <c r="Y138" s="20"/>
+      <c r="Z138" s="20"/>
+      <c r="AA138" s="20"/>
+      <c r="AB138" s="20"/>
+      <c r="AC138" s="20"/>
+      <c r="AD138" s="20"/>
+      <c r="AE138" s="20"/>
+      <c r="AF138" s="20"/>
+      <c r="AG138" s="20"/>
+      <c r="AH138" s="20"/>
+    </row>
+    <row r="139" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -8203,8 +10375,23 @@
         <v/>
       </c>
       <c r="S139" s="4"/>
-    </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T139" s="20"/>
+      <c r="U139" s="20"/>
+      <c r="V139" s="20"/>
+      <c r="W139" s="20"/>
+      <c r="X139" s="20"/>
+      <c r="Y139" s="20"/>
+      <c r="Z139" s="20"/>
+      <c r="AA139" s="20"/>
+      <c r="AB139" s="20"/>
+      <c r="AC139" s="20"/>
+      <c r="AD139" s="20"/>
+      <c r="AE139" s="20"/>
+      <c r="AF139" s="20"/>
+      <c r="AG139" s="20"/>
+      <c r="AH139" s="20"/>
+    </row>
+    <row r="140" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -8245,8 +10432,23 @@
         <v/>
       </c>
       <c r="S140" s="4"/>
-    </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T140" s="20"/>
+      <c r="U140" s="20"/>
+      <c r="V140" s="20"/>
+      <c r="W140" s="20"/>
+      <c r="X140" s="20"/>
+      <c r="Y140" s="20"/>
+      <c r="Z140" s="20"/>
+      <c r="AA140" s="20"/>
+      <c r="AB140" s="20"/>
+      <c r="AC140" s="20"/>
+      <c r="AD140" s="20"/>
+      <c r="AE140" s="20"/>
+      <c r="AF140" s="20"/>
+      <c r="AG140" s="20"/>
+      <c r="AH140" s="20"/>
+    </row>
+    <row r="141" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -8287,8 +10489,23 @@
         <v/>
       </c>
       <c r="S141" s="4"/>
-    </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T141" s="20"/>
+      <c r="U141" s="20"/>
+      <c r="V141" s="20"/>
+      <c r="W141" s="20"/>
+      <c r="X141" s="20"/>
+      <c r="Y141" s="20"/>
+      <c r="Z141" s="20"/>
+      <c r="AA141" s="20"/>
+      <c r="AB141" s="20"/>
+      <c r="AC141" s="20"/>
+      <c r="AD141" s="20"/>
+      <c r="AE141" s="20"/>
+      <c r="AF141" s="20"/>
+      <c r="AG141" s="20"/>
+      <c r="AH141" s="20"/>
+    </row>
+    <row r="142" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -8329,8 +10546,23 @@
         <v/>
       </c>
       <c r="S142" s="4"/>
-    </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T142" s="20"/>
+      <c r="U142" s="20"/>
+      <c r="V142" s="20"/>
+      <c r="W142" s="20"/>
+      <c r="X142" s="20"/>
+      <c r="Y142" s="20"/>
+      <c r="Z142" s="20"/>
+      <c r="AA142" s="20"/>
+      <c r="AB142" s="20"/>
+      <c r="AC142" s="20"/>
+      <c r="AD142" s="20"/>
+      <c r="AE142" s="20"/>
+      <c r="AF142" s="20"/>
+      <c r="AG142" s="20"/>
+      <c r="AH142" s="20"/>
+    </row>
+    <row r="143" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -8371,8 +10603,23 @@
         <v/>
       </c>
       <c r="S143" s="4"/>
-    </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T143" s="20"/>
+      <c r="U143" s="20"/>
+      <c r="V143" s="20"/>
+      <c r="W143" s="20"/>
+      <c r="X143" s="20"/>
+      <c r="Y143" s="20"/>
+      <c r="Z143" s="20"/>
+      <c r="AA143" s="20"/>
+      <c r="AB143" s="20"/>
+      <c r="AC143" s="20"/>
+      <c r="AD143" s="20"/>
+      <c r="AE143" s="20"/>
+      <c r="AF143" s="20"/>
+      <c r="AG143" s="20"/>
+      <c r="AH143" s="20"/>
+    </row>
+    <row r="144" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -8413,8 +10660,23 @@
         <v/>
       </c>
       <c r="S144" s="4"/>
-    </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T144" s="20"/>
+      <c r="U144" s="20"/>
+      <c r="V144" s="20"/>
+      <c r="W144" s="20"/>
+      <c r="X144" s="20"/>
+      <c r="Y144" s="20"/>
+      <c r="Z144" s="20"/>
+      <c r="AA144" s="20"/>
+      <c r="AB144" s="20"/>
+      <c r="AC144" s="20"/>
+      <c r="AD144" s="20"/>
+      <c r="AE144" s="20"/>
+      <c r="AF144" s="20"/>
+      <c r="AG144" s="20"/>
+      <c r="AH144" s="20"/>
+    </row>
+    <row r="145" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -8455,8 +10717,23 @@
         <v/>
       </c>
       <c r="S145" s="4"/>
-    </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T145" s="20"/>
+      <c r="U145" s="20"/>
+      <c r="V145" s="20"/>
+      <c r="W145" s="20"/>
+      <c r="X145" s="20"/>
+      <c r="Y145" s="20"/>
+      <c r="Z145" s="20"/>
+      <c r="AA145" s="20"/>
+      <c r="AB145" s="20"/>
+      <c r="AC145" s="20"/>
+      <c r="AD145" s="20"/>
+      <c r="AE145" s="20"/>
+      <c r="AF145" s="20"/>
+      <c r="AG145" s="20"/>
+      <c r="AH145" s="20"/>
+    </row>
+    <row r="146" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -8497,8 +10774,23 @@
         <v/>
       </c>
       <c r="S146" s="4"/>
-    </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T146" s="20"/>
+      <c r="U146" s="20"/>
+      <c r="V146" s="20"/>
+      <c r="W146" s="20"/>
+      <c r="X146" s="20"/>
+      <c r="Y146" s="20"/>
+      <c r="Z146" s="20"/>
+      <c r="AA146" s="20"/>
+      <c r="AB146" s="20"/>
+      <c r="AC146" s="20"/>
+      <c r="AD146" s="20"/>
+      <c r="AE146" s="20"/>
+      <c r="AF146" s="20"/>
+      <c r="AG146" s="20"/>
+      <c r="AH146" s="20"/>
+    </row>
+    <row r="147" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -8539,8 +10831,23 @@
         <v/>
       </c>
       <c r="S147" s="4"/>
-    </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T147" s="20"/>
+      <c r="U147" s="20"/>
+      <c r="V147" s="20"/>
+      <c r="W147" s="20"/>
+      <c r="X147" s="20"/>
+      <c r="Y147" s="20"/>
+      <c r="Z147" s="20"/>
+      <c r="AA147" s="20"/>
+      <c r="AB147" s="20"/>
+      <c r="AC147" s="20"/>
+      <c r="AD147" s="20"/>
+      <c r="AE147" s="20"/>
+      <c r="AF147" s="20"/>
+      <c r="AG147" s="20"/>
+      <c r="AH147" s="20"/>
+    </row>
+    <row r="148" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -8581,8 +10888,23 @@
         <v/>
       </c>
       <c r="S148" s="4"/>
-    </row>
-    <row r="149" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T148" s="20"/>
+      <c r="U148" s="20"/>
+      <c r="V148" s="20"/>
+      <c r="W148" s="20"/>
+      <c r="X148" s="20"/>
+      <c r="Y148" s="20"/>
+      <c r="Z148" s="20"/>
+      <c r="AA148" s="20"/>
+      <c r="AB148" s="20"/>
+      <c r="AC148" s="20"/>
+      <c r="AD148" s="20"/>
+      <c r="AE148" s="20"/>
+      <c r="AF148" s="20"/>
+      <c r="AG148" s="20"/>
+      <c r="AH148" s="20"/>
+    </row>
+    <row r="149" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -8623,8 +10945,23 @@
         <v/>
       </c>
       <c r="S149" s="4"/>
-    </row>
-    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T149" s="20"/>
+      <c r="U149" s="20"/>
+      <c r="V149" s="20"/>
+      <c r="W149" s="20"/>
+      <c r="X149" s="20"/>
+      <c r="Y149" s="20"/>
+      <c r="Z149" s="20"/>
+      <c r="AA149" s="20"/>
+      <c r="AB149" s="20"/>
+      <c r="AC149" s="20"/>
+      <c r="AD149" s="20"/>
+      <c r="AE149" s="20"/>
+      <c r="AF149" s="20"/>
+      <c r="AG149" s="20"/>
+      <c r="AH149" s="20"/>
+    </row>
+    <row r="150" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -8665,8 +11002,23 @@
         <v/>
       </c>
       <c r="S150" s="4"/>
-    </row>
-    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T150" s="20"/>
+      <c r="U150" s="20"/>
+      <c r="V150" s="20"/>
+      <c r="W150" s="20"/>
+      <c r="X150" s="20"/>
+      <c r="Y150" s="20"/>
+      <c r="Z150" s="20"/>
+      <c r="AA150" s="20"/>
+      <c r="AB150" s="20"/>
+      <c r="AC150" s="20"/>
+      <c r="AD150" s="20"/>
+      <c r="AE150" s="20"/>
+      <c r="AF150" s="20"/>
+      <c r="AG150" s="20"/>
+      <c r="AH150" s="20"/>
+    </row>
+    <row r="151" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -8707,8 +11059,23 @@
         <v/>
       </c>
       <c r="S151" s="4"/>
-    </row>
-    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T151" s="20"/>
+      <c r="U151" s="20"/>
+      <c r="V151" s="20"/>
+      <c r="W151" s="20"/>
+      <c r="X151" s="20"/>
+      <c r="Y151" s="20"/>
+      <c r="Z151" s="20"/>
+      <c r="AA151" s="20"/>
+      <c r="AB151" s="20"/>
+      <c r="AC151" s="20"/>
+      <c r="AD151" s="20"/>
+      <c r="AE151" s="20"/>
+      <c r="AF151" s="20"/>
+      <c r="AG151" s="20"/>
+      <c r="AH151" s="20"/>
+    </row>
+    <row r="152" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -8749,8 +11116,23 @@
         <v/>
       </c>
       <c r="S152" s="4"/>
-    </row>
-    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T152" s="20"/>
+      <c r="U152" s="20"/>
+      <c r="V152" s="20"/>
+      <c r="W152" s="20"/>
+      <c r="X152" s="20"/>
+      <c r="Y152" s="20"/>
+      <c r="Z152" s="20"/>
+      <c r="AA152" s="20"/>
+      <c r="AB152" s="20"/>
+      <c r="AC152" s="20"/>
+      <c r="AD152" s="20"/>
+      <c r="AE152" s="20"/>
+      <c r="AF152" s="20"/>
+      <c r="AG152" s="20"/>
+      <c r="AH152" s="20"/>
+    </row>
+    <row r="153" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -8791,8 +11173,23 @@
         <v/>
       </c>
       <c r="S153" s="4"/>
-    </row>
-    <row r="154" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T153" s="20"/>
+      <c r="U153" s="20"/>
+      <c r="V153" s="20"/>
+      <c r="W153" s="20"/>
+      <c r="X153" s="20"/>
+      <c r="Y153" s="20"/>
+      <c r="Z153" s="20"/>
+      <c r="AA153" s="20"/>
+      <c r="AB153" s="20"/>
+      <c r="AC153" s="20"/>
+      <c r="AD153" s="20"/>
+      <c r="AE153" s="20"/>
+      <c r="AF153" s="20"/>
+      <c r="AG153" s="20"/>
+      <c r="AH153" s="20"/>
+    </row>
+    <row r="154" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -8833,8 +11230,23 @@
         <v/>
       </c>
       <c r="S154" s="4"/>
-    </row>
-    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T154" s="20"/>
+      <c r="U154" s="20"/>
+      <c r="V154" s="20"/>
+      <c r="W154" s="20"/>
+      <c r="X154" s="20"/>
+      <c r="Y154" s="20"/>
+      <c r="Z154" s="20"/>
+      <c r="AA154" s="20"/>
+      <c r="AB154" s="20"/>
+      <c r="AC154" s="20"/>
+      <c r="AD154" s="20"/>
+      <c r="AE154" s="20"/>
+      <c r="AF154" s="20"/>
+      <c r="AG154" s="20"/>
+      <c r="AH154" s="20"/>
+    </row>
+    <row r="155" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -8875,8 +11287,23 @@
         <v/>
       </c>
       <c r="S155" s="4"/>
-    </row>
-    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T155" s="20"/>
+      <c r="U155" s="20"/>
+      <c r="V155" s="20"/>
+      <c r="W155" s="20"/>
+      <c r="X155" s="20"/>
+      <c r="Y155" s="20"/>
+      <c r="Z155" s="20"/>
+      <c r="AA155" s="20"/>
+      <c r="AB155" s="20"/>
+      <c r="AC155" s="20"/>
+      <c r="AD155" s="20"/>
+      <c r="AE155" s="20"/>
+      <c r="AF155" s="20"/>
+      <c r="AG155" s="20"/>
+      <c r="AH155" s="20"/>
+    </row>
+    <row r="156" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -8917,8 +11344,23 @@
         <v/>
       </c>
       <c r="S156" s="4"/>
-    </row>
-    <row r="157" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T156" s="20"/>
+      <c r="U156" s="20"/>
+      <c r="V156" s="20"/>
+      <c r="W156" s="20"/>
+      <c r="X156" s="20"/>
+      <c r="Y156" s="20"/>
+      <c r="Z156" s="20"/>
+      <c r="AA156" s="20"/>
+      <c r="AB156" s="20"/>
+      <c r="AC156" s="20"/>
+      <c r="AD156" s="20"/>
+      <c r="AE156" s="20"/>
+      <c r="AF156" s="20"/>
+      <c r="AG156" s="20"/>
+      <c r="AH156" s="20"/>
+    </row>
+    <row r="157" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -8959,8 +11401,23 @@
         <v/>
       </c>
       <c r="S157" s="4"/>
-    </row>
-    <row r="158" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T157" s="20"/>
+      <c r="U157" s="20"/>
+      <c r="V157" s="20"/>
+      <c r="W157" s="20"/>
+      <c r="X157" s="20"/>
+      <c r="Y157" s="20"/>
+      <c r="Z157" s="20"/>
+      <c r="AA157" s="20"/>
+      <c r="AB157" s="20"/>
+      <c r="AC157" s="20"/>
+      <c r="AD157" s="20"/>
+      <c r="AE157" s="20"/>
+      <c r="AF157" s="20"/>
+      <c r="AG157" s="20"/>
+      <c r="AH157" s="20"/>
+    </row>
+    <row r="158" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -9001,8 +11458,23 @@
         <v/>
       </c>
       <c r="S158" s="4"/>
-    </row>
-    <row r="159" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T158" s="20"/>
+      <c r="U158" s="20"/>
+      <c r="V158" s="20"/>
+      <c r="W158" s="20"/>
+      <c r="X158" s="20"/>
+      <c r="Y158" s="20"/>
+      <c r="Z158" s="20"/>
+      <c r="AA158" s="20"/>
+      <c r="AB158" s="20"/>
+      <c r="AC158" s="20"/>
+      <c r="AD158" s="20"/>
+      <c r="AE158" s="20"/>
+      <c r="AF158" s="20"/>
+      <c r="AG158" s="20"/>
+      <c r="AH158" s="20"/>
+    </row>
+    <row r="159" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -9043,8 +11515,23 @@
         <v/>
       </c>
       <c r="S159" s="4"/>
-    </row>
-    <row r="160" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T159" s="20"/>
+      <c r="U159" s="20"/>
+      <c r="V159" s="20"/>
+      <c r="W159" s="20"/>
+      <c r="X159" s="20"/>
+      <c r="Y159" s="20"/>
+      <c r="Z159" s="20"/>
+      <c r="AA159" s="20"/>
+      <c r="AB159" s="20"/>
+      <c r="AC159" s="20"/>
+      <c r="AD159" s="20"/>
+      <c r="AE159" s="20"/>
+      <c r="AF159" s="20"/>
+      <c r="AG159" s="20"/>
+      <c r="AH159" s="20"/>
+    </row>
+    <row r="160" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -9085,8 +11572,23 @@
         <v/>
       </c>
       <c r="S160" s="4"/>
-    </row>
-    <row r="161" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T160" s="20"/>
+      <c r="U160" s="20"/>
+      <c r="V160" s="20"/>
+      <c r="W160" s="20"/>
+      <c r="X160" s="20"/>
+      <c r="Y160" s="20"/>
+      <c r="Z160" s="20"/>
+      <c r="AA160" s="20"/>
+      <c r="AB160" s="20"/>
+      <c r="AC160" s="20"/>
+      <c r="AD160" s="20"/>
+      <c r="AE160" s="20"/>
+      <c r="AF160" s="20"/>
+      <c r="AG160" s="20"/>
+      <c r="AH160" s="20"/>
+    </row>
+    <row r="161" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -9127,8 +11629,23 @@
         <v/>
       </c>
       <c r="S161" s="4"/>
-    </row>
-    <row r="162" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T161" s="20"/>
+      <c r="U161" s="20"/>
+      <c r="V161" s="20"/>
+      <c r="W161" s="20"/>
+      <c r="X161" s="20"/>
+      <c r="Y161" s="20"/>
+      <c r="Z161" s="20"/>
+      <c r="AA161" s="20"/>
+      <c r="AB161" s="20"/>
+      <c r="AC161" s="20"/>
+      <c r="AD161" s="20"/>
+      <c r="AE161" s="20"/>
+      <c r="AF161" s="20"/>
+      <c r="AG161" s="20"/>
+      <c r="AH161" s="20"/>
+    </row>
+    <row r="162" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -9169,8 +11686,23 @@
         <v/>
       </c>
       <c r="S162" s="4"/>
-    </row>
-    <row r="163" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T162" s="20"/>
+      <c r="U162" s="20"/>
+      <c r="V162" s="20"/>
+      <c r="W162" s="20"/>
+      <c r="X162" s="20"/>
+      <c r="Y162" s="20"/>
+      <c r="Z162" s="20"/>
+      <c r="AA162" s="20"/>
+      <c r="AB162" s="20"/>
+      <c r="AC162" s="20"/>
+      <c r="AD162" s="20"/>
+      <c r="AE162" s="20"/>
+      <c r="AF162" s="20"/>
+      <c r="AG162" s="20"/>
+      <c r="AH162" s="20"/>
+    </row>
+    <row r="163" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A163" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -9211,8 +11743,23 @@
         <v/>
       </c>
       <c r="S163" s="4"/>
-    </row>
-    <row r="164" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T163" s="20"/>
+      <c r="U163" s="20"/>
+      <c r="V163" s="20"/>
+      <c r="W163" s="20"/>
+      <c r="X163" s="20"/>
+      <c r="Y163" s="20"/>
+      <c r="Z163" s="20"/>
+      <c r="AA163" s="20"/>
+      <c r="AB163" s="20"/>
+      <c r="AC163" s="20"/>
+      <c r="AD163" s="20"/>
+      <c r="AE163" s="20"/>
+      <c r="AF163" s="20"/>
+      <c r="AG163" s="20"/>
+      <c r="AH163" s="20"/>
+    </row>
+    <row r="164" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -9253,8 +11800,23 @@
         <v/>
       </c>
       <c r="S164" s="4"/>
-    </row>
-    <row r="165" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T164" s="20"/>
+      <c r="U164" s="20"/>
+      <c r="V164" s="20"/>
+      <c r="W164" s="20"/>
+      <c r="X164" s="20"/>
+      <c r="Y164" s="20"/>
+      <c r="Z164" s="20"/>
+      <c r="AA164" s="20"/>
+      <c r="AB164" s="20"/>
+      <c r="AC164" s="20"/>
+      <c r="AD164" s="20"/>
+      <c r="AE164" s="20"/>
+      <c r="AF164" s="20"/>
+      <c r="AG164" s="20"/>
+      <c r="AH164" s="20"/>
+    </row>
+    <row r="165" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -9295,8 +11857,23 @@
         <v/>
       </c>
       <c r="S165" s="4"/>
-    </row>
-    <row r="166" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T165" s="20"/>
+      <c r="U165" s="20"/>
+      <c r="V165" s="20"/>
+      <c r="W165" s="20"/>
+      <c r="X165" s="20"/>
+      <c r="Y165" s="20"/>
+      <c r="Z165" s="20"/>
+      <c r="AA165" s="20"/>
+      <c r="AB165" s="20"/>
+      <c r="AC165" s="20"/>
+      <c r="AD165" s="20"/>
+      <c r="AE165" s="20"/>
+      <c r="AF165" s="20"/>
+      <c r="AG165" s="20"/>
+      <c r="AH165" s="20"/>
+    </row>
+    <row r="166" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A166" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -9337,8 +11914,23 @@
         <v/>
       </c>
       <c r="S166" s="4"/>
-    </row>
-    <row r="167" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T166" s="20"/>
+      <c r="U166" s="20"/>
+      <c r="V166" s="20"/>
+      <c r="W166" s="20"/>
+      <c r="X166" s="20"/>
+      <c r="Y166" s="20"/>
+      <c r="Z166" s="20"/>
+      <c r="AA166" s="20"/>
+      <c r="AB166" s="20"/>
+      <c r="AC166" s="20"/>
+      <c r="AD166" s="20"/>
+      <c r="AE166" s="20"/>
+      <c r="AF166" s="20"/>
+      <c r="AG166" s="20"/>
+      <c r="AH166" s="20"/>
+    </row>
+    <row r="167" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -9379,8 +11971,23 @@
         <v/>
       </c>
       <c r="S167" s="4"/>
-    </row>
-    <row r="168" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T167" s="20"/>
+      <c r="U167" s="20"/>
+      <c r="V167" s="20"/>
+      <c r="W167" s="20"/>
+      <c r="X167" s="20"/>
+      <c r="Y167" s="20"/>
+      <c r="Z167" s="20"/>
+      <c r="AA167" s="20"/>
+      <c r="AB167" s="20"/>
+      <c r="AC167" s="20"/>
+      <c r="AD167" s="20"/>
+      <c r="AE167" s="20"/>
+      <c r="AF167" s="20"/>
+      <c r="AG167" s="20"/>
+      <c r="AH167" s="20"/>
+    </row>
+    <row r="168" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="str">
         <f t="shared" si="14"/>
         <v/>
@@ -9421,6 +12028,21 @@
         <v/>
       </c>
       <c r="S168" s="4"/>
+      <c r="T168" s="20"/>
+      <c r="U168" s="20"/>
+      <c r="V168" s="20"/>
+      <c r="W168" s="20"/>
+      <c r="X168" s="20"/>
+      <c r="Y168" s="20"/>
+      <c r="Z168" s="20"/>
+      <c r="AA168" s="20"/>
+      <c r="AB168" s="20"/>
+      <c r="AC168" s="20"/>
+      <c r="AD168" s="20"/>
+      <c r="AE168" s="20"/>
+      <c r="AF168" s="20"/>
+      <c r="AG168" s="20"/>
+      <c r="AH168" s="20"/>
     </row>
   </sheetData>
   <dataValidations count="6">
@@ -15677,8 +18299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A84E41FD-B4E9-444B-A54C-D5ADAA997815}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15858,15 +18480,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101007F6D915BEE4E844FB48C3AE514D89089" ma:contentTypeVersion="10" ma:contentTypeDescription="Vytvoří nový dokument" ma:contentTypeScope="" ma:versionID="d4ba2a939a563b1bbfc9e4824525ecf9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f7ae4a0-3828-4c27-918b-e30655340dac" xmlns:ns3="15216789-4c43-43b8-8f31-b3ff70bf4c88" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4c2e2fc7f2dd948a6f921154beffe86e" ns2:_="" ns3:_="">
     <xsd:import namespace="6f7ae4a0-3828-4c27-918b-e30655340dac"/>
@@ -16069,6 +18682,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -16076,14 +18698,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5159F23-DFEF-4DAD-AFD9-35AA3ABD48FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42B4D896-6DC2-4F3D-AD63-C8A6A3E9E773}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16102,6 +18716,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5159F23-DFEF-4DAD-AFD9-35AA3ABD48FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEAB0EC7-3D52-4496-A75B-1E8C2D12B388}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
PH - Zápis do excelu dle parametru
</commit_message>
<xml_diff>
--- a/data/DataSet_vyplněný.xlsx
+++ b/data/DataSet_vyplněný.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hladilpet\Documents\UiPath\PPP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7090861-9CB5-4878-84AF-6E6309ED1C4D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E13B566-1F73-4D28-8571-C26C92E248C0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27285" yWindow="45" windowWidth="28665" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vstupniData" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="614">
   <si>
     <t>No.</t>
   </si>
@@ -1877,6 +1877,15 @@
   </si>
   <si>
     <t>Výsledek zpracování</t>
+  </si>
+  <si>
+    <t>Číslo výrobního odběrného místa</t>
+  </si>
+  <si>
+    <t>TKD kontakt</t>
+  </si>
+  <si>
+    <t>Hodnota smluvního účtu</t>
   </si>
 </sst>
 </file>
@@ -1982,7 +1991,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2010,6 +2019,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
@@ -2308,10 +2318,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:AH168"/>
+  <dimension ref="A1:AK168"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC7" sqref="A1:AC7"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2339,7 +2349,7 @@
     <col min="23" max="34" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2427,21 +2437,30 @@
       <c r="AC1" s="21" t="s">
         <v>609</v>
       </c>
-      <c r="AD1" s="17" t="s">
+      <c r="AD1" s="23" t="s">
+        <v>611</v>
+      </c>
+      <c r="AE1" s="23" t="s">
+        <v>612</v>
+      </c>
+      <c r="AF1" s="23" t="s">
+        <v>613</v>
+      </c>
+      <c r="AG1" s="17" t="s">
         <v>597</v>
       </c>
-      <c r="AE1" s="17" t="s">
+      <c r="AH1" s="17" t="s">
         <v>598</v>
       </c>
-      <c r="AF1" s="17" t="s">
+      <c r="AI1" s="17" t="s">
         <v>599</v>
       </c>
-      <c r="AG1" s="22" t="s">
+      <c r="AJ1" s="22" t="s">
         <v>610</v>
       </c>
-      <c r="AH1" s="18"/>
-    </row>
-    <row r="2" spans="1:34" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AK1" s="18"/>
+    </row>
+    <row r="2" spans="1:37" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <f>IF(C2&lt;&gt;"",1,"")</f>
         <v>1</v>
@@ -2522,7 +2541,7 @@
       <c r="AG2" s="19"/>
       <c r="AH2" s="19"/>
     </row>
-    <row r="3" spans="1:34" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <f>IF(C3&lt;&gt;"",A2+1,"")</f>
         <v>2</v>
@@ -2603,7 +2622,7 @@
       <c r="AG3" s="19"/>
       <c r="AH3" s="19"/>
     </row>
-    <row r="4" spans="1:34" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <f t="shared" ref="A4:A8" si="2">IF(C4&lt;&gt;"",A3+1,"")</f>
         <v>3</v>
@@ -2684,7 +2703,7 @@
       <c r="AG4" s="19"/>
       <c r="AH4" s="19"/>
     </row>
-    <row r="5" spans="1:34" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -2760,12 +2779,9 @@
       <c r="AB5" s="19"/>
       <c r="AC5" s="19"/>
       <c r="AD5" s="19"/>
-      <c r="AE5" s="19"/>
-      <c r="AF5" s="19"/>
-      <c r="AG5" s="19"/>
       <c r="AH5" s="19"/>
     </row>
-    <row r="6" spans="1:34" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -2846,7 +2862,7 @@
       <c r="AG6" s="19"/>
       <c r="AH6" s="19"/>
     </row>
-    <row r="7" spans="1:34" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2885,7 +2901,7 @@
       <c r="AG7" s="19"/>
       <c r="AH7" s="19"/>
     </row>
-    <row r="8" spans="1:34" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2924,7 +2940,7 @@
       <c r="AG8" s="19"/>
       <c r="AH8" s="19"/>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="str">
         <f>IF(C9&lt;&gt;"",#REF!+1,"")</f>
         <v/>
@@ -2981,7 +2997,7 @@
       <c r="AG9" s="20"/>
       <c r="AH9" s="20"/>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="str">
         <f t="shared" ref="A10:A66" si="5">IF(C10&lt;&gt;"",A9+1,"")</f>
         <v/>
@@ -3038,7 +3054,7 @@
       <c r="AG10" s="20"/>
       <c r="AH10" s="20"/>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3095,7 +3111,7 @@
       <c r="AG11" s="20"/>
       <c r="AH11" s="20"/>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3152,7 +3168,7 @@
       <c r="AG12" s="20"/>
       <c r="AH12" s="20"/>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3209,7 +3225,7 @@
       <c r="AG13" s="20"/>
       <c r="AH13" s="20"/>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3266,7 +3282,7 @@
       <c r="AG14" s="20"/>
       <c r="AH14" s="20"/>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3323,7 +3339,7 @@
       <c r="AG15" s="20"/>
       <c r="AH15" s="20"/>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>

</xml_diff>

<commit_message>
oprava L3_excel_writeDataToXlsx + final L3_SAP_zalozitSmluvniUcet
</commit_message>
<xml_diff>
--- a/data/DataSet_vyplněný.xlsx
+++ b/data/DataSet_vyplněný.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hladilpet\Documents\UiPath\PPP\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hlava\Documents\UiPath\PPP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB4823A-8935-4BB2-A48E-AD49E9FDE3B5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA430CC-1AC0-4A22-8152-47436C8E56E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28935" yWindow="45" windowWidth="28665" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-210" yWindow="16080" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vstupniData" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -44,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="645">
   <si>
     <t>No.</t>
   </si>
@@ -1976,6 +1979,9 @@
   </si>
   <si>
     <t>KPJM</t>
+  </si>
+  <si>
+    <t>křemílek</t>
   </si>
 </sst>
 </file>
@@ -2138,12 +2144,14 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="List1"/>
+      <sheetName val="DoplněkUDF"/>
     </sheetNames>
     <definedNames>
       <definedName name="ConcatenateIf"/>
     </definedNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2415,8 +2423,8 @@
   <sheetPr codeName="List1"/>
   <dimension ref="A1:AL168"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3189,7 +3197,9 @@
       <c r="X10" s="20"/>
       <c r="Y10" s="20"/>
       <c r="Z10" s="20"/>
-      <c r="AA10" s="20"/>
+      <c r="AA10" s="20" t="s">
+        <v>644</v>
+      </c>
       <c r="AB10" s="20"/>
       <c r="AC10" s="20"/>
       <c r="AD10" s="20"/>
@@ -19042,6 +19052,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101007F6D915BEE4E844FB48C3AE514D89089" ma:contentTypeVersion="10" ma:contentTypeDescription="Vytvoří nový dokument" ma:contentTypeScope="" ma:versionID="d4ba2a939a563b1bbfc9e4824525ecf9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f7ae4a0-3828-4c27-918b-e30655340dac" xmlns:ns3="15216789-4c43-43b8-8f31-b3ff70bf4c88" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4c2e2fc7f2dd948a6f921154beffe86e" ns2:_="" ns3:_="">
     <xsd:import namespace="6f7ae4a0-3828-4c27-918b-e30655340dac"/>
@@ -19244,22 +19269,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5159F23-DFEF-4DAD-AFD9-35AA3ABD48FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEAB0EC7-3D52-4496-A75B-1E8C2D12B388}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42B4D896-6DC2-4F3D-AD63-C8A6A3E9E773}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19276,21 +19303,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEAB0EC7-3D52-4496-A75B-1E8C2D12B388}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5159F23-DFEF-4DAD-AFD9-35AA3ABD48FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
zapis statusu zpracovani k polozce
</commit_message>
<xml_diff>
--- a/data/DataSet_vyplněný.xlsx
+++ b/data/DataSet_vyplněný.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hlava\Documents\UiPath\PPP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51661E7D-5414-4C6E-A955-FDABD9EE39E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF973119-F8E7-4E27-8FFF-F1309F908073}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-210" yWindow="16080" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vstupniData" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="642">
   <si>
     <t>No.</t>
   </si>
@@ -1840,15 +1840,6 @@
     <t>cisloZOP</t>
   </si>
   <si>
-    <t>stav procesu 1</t>
-  </si>
-  <si>
-    <t>stav procesu2</t>
-  </si>
-  <si>
-    <t>stav procesu3</t>
-  </si>
-  <si>
     <t>doplneni 4</t>
   </si>
   <si>
@@ -1870,9 +1861,6 @@
     <t>PI</t>
   </si>
   <si>
-    <t>Výsledek zpracování</t>
-  </si>
-  <si>
     <t>Číslo výrobního odběrného místa</t>
   </si>
   <si>
@@ -1979,6 +1967,12 @@
   </si>
   <si>
     <t>KPJM</t>
+  </si>
+  <si>
+    <t>Robot - STATUS</t>
+  </si>
+  <si>
+    <t>Robot - datum poslední aktualizace</t>
   </si>
 </sst>
 </file>
@@ -2013,7 +2007,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2035,12 +2029,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2084,7 +2072,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2111,7 +2099,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2418,10 +2405,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:AL168"/>
+  <dimension ref="A1:AJ168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AD13" sqref="AD13"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AJ1" sqref="AJ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2456,12 +2443,11 @@
     <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="11" customWidth="1"/>
-    <col min="34" max="34" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="23.5703125" customWidth="1"/>
+    <col min="35" max="35" width="32.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2520,62 +2506,56 @@
         <v>572</v>
       </c>
       <c r="T1" s="18" t="s">
+        <v>636</v>
+      </c>
+      <c r="U1" s="18" t="s">
+        <v>637</v>
+      </c>
+      <c r="V1" s="18" t="s">
+        <v>639</v>
+      </c>
+      <c r="W1" s="18" t="s">
+        <v>597</v>
+      </c>
+      <c r="X1" s="21" t="s">
+        <v>598</v>
+      </c>
+      <c r="Y1" s="21" t="s">
+        <v>599</v>
+      </c>
+      <c r="Z1" s="21" t="s">
+        <v>600</v>
+      </c>
+      <c r="AA1" s="21" t="s">
+        <v>601</v>
+      </c>
+      <c r="AB1" s="21" t="s">
+        <v>602</v>
+      </c>
+      <c r="AC1" s="21" t="s">
+        <v>603</v>
+      </c>
+      <c r="AD1" s="22" t="s">
+        <v>604</v>
+      </c>
+      <c r="AE1" s="22" t="s">
+        <v>605</v>
+      </c>
+      <c r="AF1" s="22" t="s">
+        <v>606</v>
+      </c>
+      <c r="AG1" s="22" t="s">
+        <v>638</v>
+      </c>
+      <c r="AH1" s="17" t="s">
         <v>640</v>
       </c>
-      <c r="U1" s="18" t="s">
+      <c r="AI1" s="17" t="s">
         <v>641</v>
       </c>
-      <c r="V1" s="18" t="s">
-        <v>643</v>
-      </c>
-      <c r="W1" s="18" t="s">
-        <v>600</v>
-      </c>
-      <c r="X1" s="21" t="s">
-        <v>601</v>
-      </c>
-      <c r="Y1" s="21" t="s">
-        <v>602</v>
-      </c>
-      <c r="Z1" s="21" t="s">
-        <v>603</v>
-      </c>
-      <c r="AA1" s="21" t="s">
-        <v>604</v>
-      </c>
-      <c r="AB1" s="21" t="s">
-        <v>605</v>
-      </c>
-      <c r="AC1" s="21" t="s">
-        <v>606</v>
-      </c>
-      <c r="AD1" s="23" t="s">
-        <v>608</v>
-      </c>
-      <c r="AE1" s="23" t="s">
-        <v>609</v>
-      </c>
-      <c r="AF1" s="23" t="s">
-        <v>610</v>
-      </c>
-      <c r="AG1" s="23" t="s">
-        <v>642</v>
-      </c>
-      <c r="AH1" s="17" t="s">
-        <v>597</v>
-      </c>
-      <c r="AI1" s="17" t="s">
-        <v>598</v>
-      </c>
-      <c r="AJ1" s="17" t="s">
-        <v>599</v>
-      </c>
-      <c r="AK1" s="22" t="s">
-        <v>607</v>
-      </c>
-      <c r="AL1" s="18"/>
-    </row>
-    <row r="2" spans="1:38" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AJ1" s="18"/>
+    </row>
+    <row r="2" spans="1:36" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <f>IF(C2&lt;&gt;"",1,"")</f>
         <v>1</v>
@@ -2664,19 +2644,19 @@
 326 00 PLZEŇ
 www.cezdistribuce.cz/dodavatel</v>
       </c>
-      <c r="U2" s="26" t="str">
+      <c r="U2" s="25" t="str">
         <f>"PPP + osazení 4Q elměru pro novou FVE " &amp; M2 &amp; ", HJ stáv. " &amp;AB2 &amp;" A, sazba " &amp; AG2 &amp;", Pi "&amp; AC2 &amp;" kW, HDO ANO, KO č. " &amp; D2 &amp;" , "&amp; X2 &amp; ", " &amp; S2</f>
         <v>PPP + osazení 4Q elměru pro novou FVE MS, HJ stáv. 23 A, sazba , Pi 4 kW, HDO ANO, KO č. 1107959414 , Petr Hladil, 777875678</v>
       </c>
       <c r="V2" s="19"/>
       <c r="W2" s="19"/>
       <c r="X2" s="19" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="Y2" s="19" t="s">
-        <v>639</v>
-      </c>
-      <c r="Z2" s="24">
+        <v>635</v>
+      </c>
+      <c r="Z2" s="23">
         <v>31897</v>
       </c>
       <c r="AA2" s="19"/>
@@ -2693,7 +2673,7 @@
       <c r="AH2" s="19"/>
       <c r="AI2" s="19"/>
     </row>
-    <row r="3" spans="1:38" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <f>IF(C3&lt;&gt;"",A2+1,"")</f>
         <v>2</v>
@@ -2775,7 +2755,7 @@
       <c r="AH3" s="19"/>
       <c r="AI3" s="19"/>
     </row>
-    <row r="4" spans="1:38" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <f t="shared" ref="A4:A8" si="2">IF(C4&lt;&gt;"",A3+1,"")</f>
         <v>3</v>
@@ -2843,7 +2823,7 @@
       <c r="T4" s="19"/>
       <c r="U4" s="19"/>
       <c r="V4" s="19"/>
-      <c r="W4" s="25"/>
+      <c r="W4" s="24"/>
       <c r="X4" s="19"/>
       <c r="Y4" s="19"/>
       <c r="Z4" s="19"/>
@@ -2857,7 +2837,7 @@
       <c r="AH4" s="19"/>
       <c r="AI4" s="19"/>
     </row>
-    <row r="5" spans="1:38" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -2935,7 +2915,7 @@
       <c r="AD5" s="19"/>
       <c r="AI5" s="19"/>
     </row>
-    <row r="6" spans="1:38" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -3017,7 +2997,7 @@
       <c r="AH6" s="19"/>
       <c r="AI6" s="19"/>
     </row>
-    <row r="7" spans="1:38" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3057,7 +3037,7 @@
       <c r="AH7" s="19"/>
       <c r="AI7" s="19"/>
     </row>
-    <row r="8" spans="1:38" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3097,7 +3077,7 @@
       <c r="AH8" s="19"/>
       <c r="AI8" s="19"/>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="str">
         <f>IF(C9&lt;&gt;"",#REF!+1,"")</f>
         <v/>
@@ -3155,7 +3135,7 @@
       <c r="AH9" s="20"/>
       <c r="AI9" s="20"/>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="str">
         <f t="shared" ref="A10:A66" si="5">IF(C10&lt;&gt;"",A9+1,"")</f>
         <v/>
@@ -3213,7 +3193,7 @@
       <c r="AH10" s="20"/>
       <c r="AI10" s="20"/>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3271,7 +3251,7 @@
       <c r="AH11" s="20"/>
       <c r="AI11" s="20"/>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3329,7 +3309,7 @@
       <c r="AH12" s="20"/>
       <c r="AI12" s="20"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3387,7 +3367,7 @@
       <c r="AH13" s="20"/>
       <c r="AI13" s="20"/>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3445,7 +3425,7 @@
       <c r="AH14" s="20"/>
       <c r="AI14" s="20"/>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3503,7 +3483,7 @@
       <c r="AH15" s="20"/>
       <c r="AI15" s="20"/>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -18808,7 +18788,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="B21" t="str">
         <f>""""&amp; A21 &amp;": " &amp;""""&amp;"&amp; "&amp; A21&amp;".ToString" &amp; " &amp; vbcrlf &amp;"</f>
@@ -18817,7 +18797,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" ref="B22:B47" si="1">""""&amp; A22 &amp;": " &amp;""""&amp;"&amp; "&amp; A22&amp;".ToString" &amp; " &amp; vbcrlf &amp;"</f>
@@ -18826,7 +18806,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="1"/>
@@ -18835,7 +18815,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="1"/>
@@ -18844,7 +18824,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="1"/>
@@ -18853,7 +18833,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="1"/>
@@ -18862,7 +18842,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="B27" t="str">
         <f t="shared" si="1"/>
@@ -18871,7 +18851,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="1"/>
@@ -18880,7 +18860,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="B29" t="str">
         <f t="shared" si="1"/>
@@ -18889,7 +18869,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="1"/>
@@ -18898,7 +18878,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="B31" t="str">
         <f t="shared" si="1"/>
@@ -18907,7 +18887,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="B32" t="str">
         <f t="shared" si="1"/>
@@ -18916,7 +18896,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" si="1"/>
@@ -18925,7 +18905,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" si="1"/>
@@ -18934,7 +18914,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="1"/>
@@ -18943,7 +18923,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="1"/>
@@ -18952,7 +18932,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="1"/>
@@ -18961,7 +18941,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="1"/>
@@ -18970,7 +18950,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="1"/>
@@ -18979,7 +18959,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="1"/>
@@ -18988,7 +18968,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="1"/>
@@ -18997,7 +18977,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="1"/>
@@ -19006,7 +18986,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="B43" t="str">
         <f t="shared" si="1"/>
@@ -19015,7 +18995,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="B44" t="str">
         <f t="shared" si="1"/>
@@ -19024,7 +19004,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="1"/>
@@ -19033,7 +19013,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="1"/>
@@ -19042,7 +19022,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="B47" t="str">
         <f t="shared" si="1"/>
@@ -19056,21 +19036,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101007F6D915BEE4E844FB48C3AE514D89089" ma:contentTypeVersion="10" ma:contentTypeDescription="Vytvoří nový dokument" ma:contentTypeScope="" ma:versionID="d4ba2a939a563b1bbfc9e4824525ecf9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f7ae4a0-3828-4c27-918b-e30655340dac" xmlns:ns3="15216789-4c43-43b8-8f31-b3ff70bf4c88" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4c2e2fc7f2dd948a6f921154beffe86e" ns2:_="" ns3:_="">
     <xsd:import namespace="6f7ae4a0-3828-4c27-918b-e30655340dac"/>
@@ -19273,24 +19238,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5159F23-DFEF-4DAD-AFD9-35AA3ABD48FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEAB0EC7-3D52-4496-A75B-1E8C2D12B388}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42B4D896-6DC2-4F3D-AD63-C8A6A3E9E773}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19307,4 +19270,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEAB0EC7-3D52-4496-A75B-1E8C2D12B388}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5159F23-DFEF-4DAD-AFD9-35AA3ABD48FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>